<commit_message>
[feat][resource-server][Add JWT symmetric key]
</commit_message>
<xml_diff>
--- a/Doc/Documents.xlsx
+++ b/Doc/Documents.xlsx
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="776" uniqueCount="757">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="780" uniqueCount="761">
   <si>
     <t>Kiến Trúc về Microservice</t>
   </si>
@@ -3726,13 +3726,6 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
       <t xml:space="preserve"> - JSON: It uses JSON to format the data it contains.
  - WEB: It’s designed to be used for web requests.
  - TOKEN: It’s a token implementation.
@@ -3823,7 +3816,84 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> graphic algorithm
-   + Digital signature(): This part can be missing</t>
+   + Digital signature(): This part can be missing
+- A JWT is a token implementation. A token consists of three parts: the header, the body, and the signature. The details in the header and the body are represented with JSON, and they are Base64 encoded. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">The third part is the signature, generated using a cryptographic algorithm that uses as input the header and the body
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">- The cryptographic algorithm also implies the need for a key. The key is like a password. Someone having a proper key can sign a token or validate that a signature is authentic. If the signature on a token is authentic, that guarantees that nobody altered the token after it was signed.
+- If a hacker sees the contents in the token, they can’t change a token’s contents because if they do so, the signature becomes invalid. To be valid, a </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>signature</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> has to: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Be generated with the correct key</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Match the content that was signed</t>
     </r>
   </si>
   <si>
@@ -4767,35 +4837,62 @@
     <t>Reseource Server</t>
   </si>
   <si>
-    <t>The first option allows the resource server to directly call the authorization server to verify an issued token:
+    <r>
+      <t>1. The first option</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> allows the resource server to directly call the authorization server to verify an issued token:
  - After obtaining a token from the autohrization server, the client calls the endpoints exposed bu the resouce server
  - To validate the access token received from the client, the resource server directly calls the authorization server
  - Easy to implement. It can be applied to any token implementation.
  - It implies direct dependency between the authorization server and the resource server. It might cause unnecessary stress on the authorization server.</t>
-  </si>
-  <si>
-    <t>The second option(blackboarding) 
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>2. The second option(blackboarding)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 
  - uses a common database where the authorization server stores tokens, and then the resource server can access and validate the tokens
  - Eliminates the need for direct communication between the authorization server and the resource server.It’s more difficult to implement than directly calling the authorization server.
  - It can be applied to any token implementation.Requires one more component in the system, the shared database.
  - Persisting tokens allows authorization to work after an authorization server restart or if the authorization server is down.</t>
-  </si>
-  <si>
-    <r>
-      <t>The third option uses cryptographic signatures</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>:
- - The authorization server signs the token when issuing it, and the resource server validates the signature. Here’s where we generally use JSON Web Tokens (JWTs)
- - Allowing the resource server to validate them without needing to call the authorization server directly and without needing a shared database.</t>
-    </r>
+    </r>
+  </si>
+  <si>
+    <t>3. The third option uses cryptographic signatures</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - The authorization server signs the token when issuing it, and the resource server validates the signature. Here’s where we generally use JSON Web Tokens (JWTs)
+ - Allowing the resource server to validate them without needing to call the authorization server directly and without needing a shared database.
+ - JWT</t>
+  </si>
+  <si>
+    <t>3.1: Using tokens signed with symmetric(đối xứng) keys with JWT
+ - Using the same key, you can both sign a token and validate its signature.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.2: Using tokens signed with asymmetric(bất đối xứng) keys with JWT
+ - </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.3: Adding custom details to the JWT
+ - </t>
   </si>
   <si>
     <t>JDBC là gì?</t>
@@ -9194,10 +9291,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="36">
     <font>
@@ -9315,24 +9412,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -9346,8 +9435,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -9358,6 +9448,29 @@
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -9376,9 +9489,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -9393,7 +9512,7 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -9401,29 +9520,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -9522,25 +9619,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -9558,6 +9667,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -9570,7 +9685,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -9582,19 +9715,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -9606,19 +9727,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -9630,61 +9775,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -9778,16 +9875,22 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -9803,6 +9906,17 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -9824,10 +9938,8 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -9841,135 +9953,120 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="12" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="13" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="15" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="12" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -9979,16 +10076,16 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -9996,7 +10093,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="48"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -10139,12 +10236,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -10864,7 +10955,7 @@
       <c r="B1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="84" t="s">
+      <c r="C1" s="82" t="s">
         <v>1</v>
       </c>
     </row>
@@ -10875,7 +10966,7 @@
       <c r="B2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="84" t="s">
+      <c r="C2" s="82" t="s">
         <v>3</v>
       </c>
     </row>
@@ -10883,10 +10974,10 @@
       <c r="A3" s="7">
         <v>3</v>
       </c>
-      <c r="B3" s="82" t="s">
+      <c r="B3" s="80" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="84" t="s">
+      <c r="C3" s="82" t="s">
         <v>5</v>
       </c>
     </row>
@@ -10897,7 +10988,7 @@
       <c r="B4" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="85" t="s">
+      <c r="C4" s="83" t="s">
         <v>7</v>
       </c>
     </row>
@@ -10919,7 +11010,7 @@
       <c r="B6" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="85" t="s">
+      <c r="C6" s="83" t="s">
         <v>11</v>
       </c>
     </row>
@@ -10930,7 +11021,7 @@
       <c r="B7" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="68" t="s">
+      <c r="C7" s="66" t="s">
         <v>13</v>
       </c>
     </row>
@@ -10941,7 +11032,7 @@
       <c r="B8" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="68" t="s">
+      <c r="C8" s="66" t="s">
         <v>15</v>
       </c>
     </row>
@@ -10952,7 +11043,7 @@
       <c r="B9" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="84" t="s">
+      <c r="C9" s="82" t="s">
         <v>17</v>
       </c>
     </row>
@@ -10966,7 +11057,7 @@
       <c r="C10" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="83" t="s">
+      <c r="D10" s="81" t="s">
         <v>20</v>
       </c>
     </row>
@@ -11001,7 +11092,7 @@
       <c r="C14" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="D14" s="68" t="s">
+      <c r="D14" s="66" t="s">
         <v>29</v>
       </c>
       <c r="E14" s="8" t="s">
@@ -11031,7 +11122,7 @@
       <c r="B17" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="C17" s="68" t="s">
+      <c r="C17" s="66" t="s">
         <v>37</v>
       </c>
     </row>
@@ -11039,7 +11130,7 @@
       <c r="B18" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="C18" s="68" t="s">
+      <c r="C18" s="66" t="s">
         <v>39</v>
       </c>
     </row>
@@ -11070,230 +11161,230 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="32" t="s">
-        <v>447</v>
+        <v>451</v>
       </c>
       <c r="B1" s="33" t="s">
-        <v>448</v>
+        <v>452</v>
       </c>
     </row>
     <row r="2" ht="38.25" spans="1:2">
       <c r="A2" t="s">
-        <v>449</v>
+        <v>453</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>450</v>
+        <v>454</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>451</v>
+        <v>455</v>
       </c>
       <c r="B3" t="s">
-        <v>452</v>
+        <v>456</v>
       </c>
     </row>
     <row r="4" ht="51" spans="1:2">
       <c r="A4" t="s">
-        <v>453</v>
+        <v>457</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>454</v>
+        <v>458</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>455</v>
+        <v>459</v>
       </c>
       <c r="B5" t="s">
-        <v>456</v>
+        <v>460</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>457</v>
+        <v>461</v>
       </c>
       <c r="B6" t="s">
-        <v>458</v>
+        <v>462</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>459</v>
+        <v>463</v>
       </c>
       <c r="B7" t="s">
-        <v>460</v>
+        <v>464</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>461</v>
+        <v>465</v>
       </c>
       <c r="B8" t="s">
-        <v>462</v>
+        <v>466</v>
       </c>
     </row>
     <row r="9" ht="63.75" spans="1:2">
       <c r="A9" t="s">
-        <v>463</v>
+        <v>467</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>464</v>
+        <v>468</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>465</v>
+        <v>469</v>
       </c>
       <c r="B10" t="s">
-        <v>466</v>
+        <v>470</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" t="s">
-        <v>467</v>
+        <v>471</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" t="s">
-        <v>468</v>
+        <v>472</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" t="s">
-        <v>469</v>
+        <v>473</v>
       </c>
     </row>
     <row r="14" ht="25.5" spans="1:2">
       <c r="A14" t="s">
-        <v>470</v>
+        <v>474</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>471</v>
+        <v>475</v>
       </c>
     </row>
     <row r="15" ht="51" spans="1:2">
       <c r="A15" t="s">
-        <v>472</v>
+        <v>476</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>473</v>
+        <v>477</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="33" t="s">
-        <v>474</v>
+        <v>478</v>
       </c>
       <c r="B16" t="s">
-        <v>475</v>
+        <v>479</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" t="s">
-        <v>476</v>
+        <v>480</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" t="s">
-        <v>477</v>
+        <v>481</v>
       </c>
     </row>
     <row r="19" ht="51" spans="1:2">
       <c r="A19" t="s">
-        <v>478</v>
+        <v>482</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>479</v>
+        <v>483</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" t="s">
-        <v>480</v>
+        <v>484</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21" t="s">
-        <v>481</v>
+        <v>485</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22" t="s">
-        <v>482</v>
+        <v>486</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>483</v>
+        <v>487</v>
       </c>
       <c r="B23" t="s">
-        <v>484</v>
+        <v>488</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>485</v>
+        <v>489</v>
       </c>
       <c r="B24" t="s">
-        <v>486</v>
+        <v>490</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>487</v>
+        <v>491</v>
       </c>
       <c r="B25" t="s">
-        <v>488</v>
+        <v>492</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" t="s">
-        <v>489</v>
+        <v>493</v>
       </c>
       <c r="B26" t="s">
-        <v>490</v>
+        <v>494</v>
       </c>
     </row>
     <row r="28" ht="63.75" spans="1:2">
       <c r="A28" s="6" t="s">
-        <v>491</v>
+        <v>495</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>492</v>
+        <v>496</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" s="6"/>
       <c r="B29" t="s">
-        <v>493</v>
+        <v>497</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" s="6"/>
       <c r="B30" t="s">
-        <v>494</v>
+        <v>498</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" s="6"/>
       <c r="B31" t="s">
-        <v>495</v>
+        <v>499</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" s="6"/>
       <c r="B32" t="s">
-        <v>496</v>
+        <v>500</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="6"/>
       <c r="B33" t="s">
-        <v>497</v>
+        <v>501</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" s="6"/>
       <c r="B34" t="s">
-        <v>498</v>
+        <v>502</v>
       </c>
     </row>
   </sheetData>
@@ -11322,195 +11413,195 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="30" t="s">
-        <v>499</v>
+        <v>503</v>
       </c>
       <c r="B1" s="31" t="s">
-        <v>500</v>
+        <v>504</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>501</v>
+        <v>505</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>502</v>
+        <v>506</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>503</v>
+        <v>507</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>504</v>
+        <v>508</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>505</v>
+        <v>509</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>506</v>
+        <v>510</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" t="s">
-        <v>507</v>
+        <v>511</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" t="s">
-        <v>508</v>
+        <v>512</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" t="s">
-        <v>509</v>
+        <v>513</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" t="s">
-        <v>510</v>
+        <v>514</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" t="s">
-        <v>511</v>
+        <v>515</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" t="s">
-        <v>512</v>
+        <v>516</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16" t="s">
-        <v>513</v>
+        <v>517</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" t="s">
-        <v>514</v>
+        <v>518</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" t="s">
-        <v>515</v>
+        <v>519</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" t="s">
-        <v>516</v>
+        <v>520</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>517</v>
+        <v>521</v>
       </c>
       <c r="B21" s="25" t="s">
-        <v>518</v>
+        <v>522</v>
       </c>
     </row>
     <row r="24" ht="63.75" spans="1:2">
       <c r="A24" t="s">
-        <v>519</v>
+        <v>523</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>520</v>
+        <v>524</v>
       </c>
     </row>
     <row r="25" ht="25.5" spans="1:2">
       <c r="A25" t="s">
-        <v>521</v>
+        <v>525</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>522</v>
+        <v>526</v>
       </c>
     </row>
     <row r="26" spans="1:1">
       <c r="A26" t="s">
-        <v>523</v>
+        <v>527</v>
       </c>
     </row>
     <row r="27" spans="1:1">
       <c r="A27" t="s">
-        <v>524</v>
+        <v>528</v>
       </c>
     </row>
     <row r="28" spans="1:1">
       <c r="A28" t="s">
-        <v>525</v>
+        <v>529</v>
       </c>
     </row>
     <row r="29" spans="1:1">
       <c r="A29" t="s">
-        <v>526</v>
+        <v>530</v>
       </c>
     </row>
     <row r="30" spans="1:1">
       <c r="A30" t="s">
-        <v>527</v>
+        <v>531</v>
       </c>
     </row>
     <row r="31" spans="1:1">
       <c r="A31" t="s">
-        <v>528</v>
+        <v>532</v>
       </c>
     </row>
     <row r="32" spans="1:1">
       <c r="A32" t="s">
-        <v>529</v>
+        <v>533</v>
       </c>
     </row>
     <row r="33" spans="1:1">
       <c r="A33" t="s">
-        <v>530</v>
+        <v>534</v>
       </c>
     </row>
     <row r="34" spans="1:1">
       <c r="A34" t="s">
-        <v>531</v>
+        <v>535</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" s="6" t="s">
-        <v>532</v>
+        <v>536</v>
       </c>
       <c r="B35" t="s">
-        <v>533</v>
+        <v>537</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" s="6"/>
       <c r="B36" t="s">
-        <v>534</v>
+        <v>538</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" s="6"/>
       <c r="B37" t="s">
-        <v>535</v>
+        <v>539</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" s="6"/>
       <c r="B38" t="s">
-        <v>536</v>
+        <v>540</v>
       </c>
     </row>
     <row r="39" spans="1:1">
       <c r="A39" t="s">
-        <v>537</v>
+        <v>541</v>
       </c>
     </row>
     <row r="40" spans="1:1">
       <c r="A40" t="s">
-        <v>538</v>
+        <v>542</v>
       </c>
     </row>
   </sheetData>
@@ -11542,140 +11633,140 @@
   <sheetData>
     <row r="1" ht="127.5" spans="1:3">
       <c r="A1" s="24" t="s">
-        <v>539</v>
-      </c>
-      <c r="B1" s="85" t="s">
-        <v>540</v>
+        <v>543</v>
+      </c>
+      <c r="B1" s="83" t="s">
+        <v>544</v>
       </c>
       <c r="C1" s="25" t="s">
-        <v>541</v>
+        <v>545</v>
       </c>
     </row>
     <row r="2" ht="200.25" customHeight="1" spans="1:2">
       <c r="A2" s="8" t="s">
-        <v>542</v>
+        <v>546</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>543</v>
+        <v>547</v>
       </c>
     </row>
     <row r="3" ht="102" spans="1:2">
       <c r="A3" s="8" t="s">
-        <v>544</v>
+        <v>548</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>545</v>
+        <v>549</v>
       </c>
     </row>
     <row r="4" ht="25.5" spans="1:2">
       <c r="A4" s="8" t="s">
-        <v>546</v>
-      </c>
-      <c r="B4" s="85" t="s">
-        <v>547</v>
+        <v>550</v>
+      </c>
+      <c r="B4" s="83" t="s">
+        <v>551</v>
       </c>
     </row>
     <row r="5" ht="25.5" spans="1:2">
       <c r="A5" s="8" t="s">
-        <v>548</v>
+        <v>552</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>549</v>
+        <v>553</v>
       </c>
     </row>
     <row r="6" ht="38.25" spans="1:1">
       <c r="A6" s="8" t="s">
-        <v>550</v>
+        <v>554</v>
       </c>
     </row>
     <row r="7" ht="38.25" spans="1:2">
       <c r="A7" s="8" t="s">
-        <v>551</v>
+        <v>555</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>552</v>
+        <v>556</v>
       </c>
     </row>
     <row r="8" ht="114.75" spans="1:2">
       <c r="A8" s="8" t="s">
-        <v>553</v>
+        <v>557</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>554</v>
+        <v>558</v>
       </c>
     </row>
     <row r="12" ht="51" spans="1:2">
       <c r="A12" s="8" t="s">
-        <v>555</v>
+        <v>559</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>556</v>
+        <v>560</v>
       </c>
     </row>
     <row r="13" ht="51" spans="1:2">
       <c r="A13" s="8" t="s">
-        <v>557</v>
+        <v>561</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>558</v>
+        <v>562</v>
       </c>
     </row>
     <row r="14" ht="89.25" spans="1:2">
       <c r="A14" s="8" t="s">
-        <v>559</v>
+        <v>563</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>560</v>
+        <v>564</v>
       </c>
     </row>
     <row r="15" ht="102" spans="1:2">
       <c r="A15" s="8" t="s">
-        <v>561</v>
+        <v>565</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>562</v>
+        <v>566</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="8" t="s">
-        <v>563</v>
+        <v>567</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>564</v>
+        <v>568</v>
       </c>
     </row>
     <row r="17" ht="178.5" spans="1:2">
       <c r="A17" s="8" t="s">
-        <v>565</v>
+        <v>569</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>566</v>
+        <v>570</v>
       </c>
     </row>
     <row r="18" ht="25.5" spans="1:2">
       <c r="A18" s="8" t="s">
-        <v>567</v>
+        <v>571</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>568</v>
+        <v>572</v>
       </c>
     </row>
     <row r="19" ht="280.5" spans="1:2">
       <c r="A19" s="8" t="s">
-        <v>569</v>
+        <v>573</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>570</v>
+        <v>574</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" s="8" t="s">
-        <v>571</v>
+        <v>575</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22" s="8" t="s">
-        <v>519</v>
+        <v>523</v>
       </c>
     </row>
     <row r="23" spans="2:2">
@@ -11683,145 +11774,145 @@
     </row>
     <row r="25" spans="1:1">
       <c r="A25" s="8" t="s">
-        <v>572</v>
+        <v>576</v>
       </c>
     </row>
     <row r="28" spans="1:1">
       <c r="A28" s="8" t="s">
-        <v>573</v>
+        <v>577</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" s="8" t="s">
-        <v>574</v>
+        <v>578</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>575</v>
+        <v>579</v>
       </c>
     </row>
     <row r="33" ht="38.25" spans="1:2">
       <c r="A33" s="8" t="s">
-        <v>576</v>
+        <v>580</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>577</v>
+        <v>581</v>
       </c>
     </row>
     <row r="34" ht="114.75" spans="1:2">
       <c r="A34" s="8" t="s">
-        <v>578</v>
+        <v>582</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>579</v>
+        <v>583</v>
       </c>
     </row>
     <row r="36" spans="1:1">
       <c r="A36" s="8" t="s">
-        <v>580</v>
+        <v>584</v>
       </c>
     </row>
     <row r="38" spans="1:1">
       <c r="A38" s="8" t="s">
-        <v>581</v>
+        <v>585</v>
       </c>
     </row>
     <row r="40" spans="1:1">
       <c r="A40" s="8" t="s">
-        <v>582</v>
+        <v>586</v>
       </c>
     </row>
     <row r="42" spans="1:1">
       <c r="A42" s="8" t="s">
-        <v>583</v>
+        <v>587</v>
       </c>
     </row>
     <row r="44" spans="1:1">
       <c r="A44" s="8" t="s">
-        <v>584</v>
+        <v>588</v>
       </c>
     </row>
     <row r="46" spans="1:1">
       <c r="A46" s="8" t="s">
-        <v>585</v>
+        <v>589</v>
       </c>
     </row>
     <row r="48" spans="1:1">
       <c r="A48" s="8" t="s">
-        <v>586</v>
+        <v>590</v>
       </c>
     </row>
     <row r="50" spans="1:1">
       <c r="A50" s="8" t="s">
-        <v>587</v>
+        <v>591</v>
       </c>
     </row>
     <row r="52" spans="1:1">
       <c r="A52" s="8" t="s">
-        <v>588</v>
+        <v>592</v>
       </c>
     </row>
     <row r="54" spans="1:2">
       <c r="A54" s="27" t="s">
-        <v>589</v>
+        <v>593</v>
       </c>
       <c r="B54" s="8" t="s">
-        <v>590</v>
+        <v>594</v>
       </c>
     </row>
     <row r="55" spans="1:2">
       <c r="A55" s="27"/>
       <c r="B55" s="8" t="s">
-        <v>591</v>
+        <v>595</v>
       </c>
     </row>
     <row r="56" spans="1:2">
       <c r="A56" s="27"/>
       <c r="B56" s="8" t="s">
-        <v>592</v>
+        <v>596</v>
       </c>
     </row>
     <row r="58" ht="25.5" spans="1:2">
       <c r="A58" s="28" t="s">
-        <v>593</v>
+        <v>597</v>
       </c>
       <c r="B58" s="8" t="s">
-        <v>594</v>
+        <v>598</v>
       </c>
     </row>
     <row r="59" spans="1:2">
       <c r="A59" s="28"/>
       <c r="B59" s="29" t="s">
-        <v>595</v>
+        <v>599</v>
       </c>
     </row>
     <row r="60" spans="1:2">
       <c r="A60" s="28"/>
       <c r="B60" s="29" t="s">
-        <v>596</v>
+        <v>600</v>
       </c>
     </row>
     <row r="61" spans="1:2">
       <c r="A61" s="28"/>
       <c r="B61" s="29" t="s">
-        <v>597</v>
+        <v>601</v>
       </c>
     </row>
     <row r="62" spans="1:2">
       <c r="A62" s="28"/>
       <c r="B62" s="29" t="s">
-        <v>598</v>
+        <v>602</v>
       </c>
     </row>
     <row r="63" spans="1:2">
       <c r="A63" s="28"/>
       <c r="B63" s="29" t="s">
-        <v>599</v>
+        <v>603</v>
       </c>
     </row>
     <row r="64" spans="1:2">
       <c r="A64" s="28"/>
       <c r="B64" s="29" t="s">
-        <v>600</v>
+        <v>604</v>
       </c>
     </row>
   </sheetData>
@@ -11854,276 +11945,276 @@
   <sheetData>
     <row r="1" ht="89.25" spans="1:2">
       <c r="A1" s="6" t="s">
-        <v>505</v>
+        <v>509</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>601</v>
+        <v>605</v>
       </c>
     </row>
     <row r="2" ht="89.25" spans="1:2">
       <c r="A2" s="6"/>
       <c r="B2" s="15" t="s">
-        <v>602</v>
+        <v>606</v>
       </c>
     </row>
     <row r="3" ht="102" spans="1:2">
       <c r="A3" s="6"/>
       <c r="B3" s="2" t="s">
-        <v>603</v>
+        <v>607</v>
       </c>
     </row>
     <row r="4" ht="63.75" spans="1:2">
       <c r="A4" s="6" t="s">
-        <v>604</v>
+        <v>608</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>605</v>
+        <v>609</v>
       </c>
     </row>
     <row r="5" ht="63.75" spans="1:2">
       <c r="A5" s="6"/>
       <c r="B5" s="15" t="s">
-        <v>606</v>
+        <v>610</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="6"/>
       <c r="B6" s="15" t="s">
-        <v>607</v>
+        <v>611</v>
       </c>
     </row>
     <row r="7" ht="38.25" spans="1:2">
       <c r="A7" s="6" t="s">
-        <v>608</v>
+        <v>612</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>609</v>
+        <v>613</v>
       </c>
     </row>
     <row r="8" ht="38.25" spans="1:2">
       <c r="A8" s="6"/>
       <c r="B8" s="15" t="s">
-        <v>610</v>
+        <v>614</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="6"/>
       <c r="B9" s="15" t="s">
-        <v>611</v>
+        <v>615</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="6"/>
       <c r="B10" s="15" t="s">
-        <v>612</v>
+        <v>616</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="6"/>
       <c r="B11" s="15" t="s">
-        <v>613</v>
+        <v>617</v>
       </c>
     </row>
     <row r="12" ht="51" spans="1:2">
       <c r="A12" s="6" t="s">
-        <v>614</v>
+        <v>618</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>615</v>
+        <v>619</v>
       </c>
     </row>
     <row r="13" ht="63.75" spans="1:2">
       <c r="A13" s="6"/>
       <c r="B13" s="15" t="s">
-        <v>616</v>
+        <v>620</v>
       </c>
     </row>
     <row r="14" ht="127.5" spans="1:2">
       <c r="A14" s="6"/>
       <c r="B14" s="15" t="s">
-        <v>617</v>
+        <v>621</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="6"/>
       <c r="B15" s="15" t="s">
-        <v>618</v>
+        <v>622</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="6"/>
       <c r="B16" s="15" t="s">
-        <v>619</v>
+        <v>623</v>
       </c>
     </row>
     <row r="17" ht="102" spans="1:2">
       <c r="A17" s="6"/>
       <c r="B17" s="15" t="s">
-        <v>620</v>
+        <v>624</v>
       </c>
     </row>
     <row r="18" ht="38.25" spans="1:2">
       <c r="A18" s="6"/>
       <c r="B18" s="15" t="s">
-        <v>621</v>
+        <v>625</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="6"/>
       <c r="B19" s="15" t="s">
-        <v>622</v>
+        <v>626</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="6"/>
       <c r="B20" s="17" t="s">
-        <v>623</v>
+        <v>627</v>
       </c>
     </row>
     <row r="21" ht="165.75" spans="1:2">
       <c r="A21" s="18" t="s">
-        <v>624</v>
+        <v>628</v>
       </c>
       <c r="B21" s="15" t="s">
-        <v>625</v>
+        <v>629</v>
       </c>
     </row>
     <row r="22" ht="242.25" spans="1:2">
       <c r="A22" s="18"/>
       <c r="B22" s="15" t="s">
-        <v>626</v>
+        <v>630</v>
       </c>
     </row>
     <row r="23" ht="153" spans="1:2">
       <c r="A23" s="18"/>
       <c r="B23" s="15" t="s">
-        <v>627</v>
+        <v>631</v>
       </c>
     </row>
     <row r="24" ht="38.25" spans="1:2">
       <c r="A24" s="18"/>
       <c r="B24" s="15" t="s">
-        <v>628</v>
+        <v>632</v>
       </c>
     </row>
     <row r="25" ht="25.5" spans="1:2">
       <c r="A25" s="18"/>
       <c r="B25" s="15" t="s">
-        <v>629</v>
+        <v>633</v>
       </c>
     </row>
     <row r="26" ht="51" spans="1:2">
       <c r="A26" s="18"/>
       <c r="B26" s="15" t="s">
-        <v>630</v>
+        <v>634</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" s="18"/>
       <c r="B27" s="15" t="s">
-        <v>631</v>
+        <v>635</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" s="18"/>
       <c r="B28" s="17" t="s">
-        <v>632</v>
+        <v>636</v>
       </c>
     </row>
     <row r="29" ht="38.25" spans="1:2">
       <c r="A29" s="22" t="s">
-        <v>633</v>
+        <v>637</v>
       </c>
       <c r="B29" s="15" t="s">
-        <v>634</v>
+        <v>638</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" s="6"/>
       <c r="B30" s="15" t="s">
-        <v>635</v>
+        <v>639</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" s="6"/>
       <c r="B31" s="15" t="s">
-        <v>636</v>
+        <v>640</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" s="6"/>
       <c r="B32" s="15" t="s">
-        <v>637</v>
+        <v>641</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="6"/>
       <c r="B33" s="15" t="s">
-        <v>638</v>
+        <v>642</v>
       </c>
     </row>
     <row r="34" ht="51" spans="1:2">
       <c r="A34" s="18" t="s">
-        <v>639</v>
+        <v>643</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>640</v>
+        <v>644</v>
       </c>
     </row>
     <row r="35" ht="38.25" spans="1:2">
       <c r="A35" s="6"/>
       <c r="B35" s="5" t="s">
-        <v>641</v>
+        <v>645</v>
       </c>
     </row>
     <row r="36" ht="51" spans="1:2">
       <c r="A36" s="6"/>
       <c r="B36" s="5" t="s">
-        <v>642</v>
+        <v>646</v>
       </c>
     </row>
     <row r="37" ht="51" spans="1:2">
       <c r="A37" s="6"/>
       <c r="B37" s="5" t="s">
-        <v>643</v>
+        <v>647</v>
       </c>
     </row>
     <row r="38" ht="25.5" spans="1:2">
       <c r="A38" s="6" t="s">
-        <v>644</v>
+        <v>648</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>645</v>
+        <v>649</v>
       </c>
     </row>
     <row r="39" ht="76.5" spans="1:2">
       <c r="A39" s="6"/>
       <c r="B39" s="2" t="s">
-        <v>646</v>
+        <v>650</v>
       </c>
     </row>
     <row r="40" ht="25.5" spans="1:2">
       <c r="A40" s="6"/>
       <c r="B40" s="2" t="s">
-        <v>647</v>
+        <v>651</v>
       </c>
     </row>
     <row r="41" ht="25.5" spans="1:2">
       <c r="A41" s="6"/>
       <c r="B41" s="2" t="s">
-        <v>648</v>
+        <v>652</v>
       </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" s="6"/>
       <c r="B42" s="2" t="s">
-        <v>649</v>
+        <v>653</v>
       </c>
     </row>
     <row r="43" ht="25.5" spans="1:2">
       <c r="A43" s="6"/>
       <c r="B43" s="2" t="s">
-        <v>650</v>
+        <v>654</v>
       </c>
     </row>
     <row r="44" spans="1:2">
@@ -12132,10 +12223,10 @@
     </row>
     <row r="45" ht="25.5" spans="1:2">
       <c r="A45" s="6" t="s">
-        <v>651</v>
+        <v>655</v>
       </c>
       <c r="B45" s="23" t="s">
-        <v>652</v>
+        <v>656</v>
       </c>
     </row>
   </sheetData>
@@ -12178,10 +12269,10 @@
   <sheetData>
     <row r="1" ht="114.75" spans="1:3">
       <c r="A1" s="12" t="s">
-        <v>653</v>
-      </c>
-      <c r="B1" s="88" t="s">
-        <v>654</v>
+        <v>657</v>
+      </c>
+      <c r="B1" s="86" t="s">
+        <v>658</v>
       </c>
       <c r="C1" s="12" t="s">
         <v>133</v>
@@ -12189,29 +12280,29 @@
     </row>
     <row r="2" ht="89.25" spans="1:2">
       <c r="A2" s="12" t="s">
-        <v>655</v>
-      </c>
-      <c r="B2" s="89" t="s">
-        <v>656</v>
+        <v>659</v>
+      </c>
+      <c r="B2" s="87" t="s">
+        <v>660</v>
       </c>
     </row>
     <row r="3" ht="63.75" spans="1:3">
       <c r="A3" s="12" t="s">
-        <v>657</v>
+        <v>661</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>658</v>
+        <v>662</v>
       </c>
       <c r="C3" s="21" t="s">
-        <v>659</v>
+        <v>663</v>
       </c>
     </row>
     <row r="4" ht="51" spans="1:2">
       <c r="A4" s="12" t="s">
-        <v>660</v>
+        <v>664</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>661</v>
+        <v>665</v>
       </c>
     </row>
   </sheetData>
@@ -12240,18 +12331,18 @@
   <sheetData>
     <row r="1" ht="89.25" spans="1:2">
       <c r="A1" s="8" t="s">
-        <v>662</v>
-      </c>
-      <c r="B1" s="85" t="s">
-        <v>663</v>
+        <v>666</v>
+      </c>
+      <c r="B1" s="83" t="s">
+        <v>667</v>
       </c>
     </row>
     <row r="2" ht="178.5" spans="1:2">
       <c r="A2" s="7" t="s">
-        <v>664</v>
+        <v>668</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>665</v>
+        <v>669</v>
       </c>
     </row>
   </sheetData>
@@ -12309,22 +12400,22 @@
   <sheetData>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>666</v>
+        <v>670</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>667</v>
+        <v>671</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>668</v>
+        <v>672</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" t="s">
-        <v>669</v>
+        <v>673</v>
       </c>
     </row>
   </sheetData>
@@ -12351,10 +12442,10 @@
   <sheetData>
     <row r="1" ht="26.25" customHeight="1" spans="1:2">
       <c r="A1" s="9" t="s">
-        <v>670</v>
+        <v>674</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>671</v>
+        <v>675</v>
       </c>
     </row>
     <row r="2" spans="1:1">
@@ -12362,120 +12453,120 @@
     </row>
     <row r="3" ht="140.25" spans="1:3">
       <c r="A3" s="11" t="s">
-        <v>672</v>
+        <v>676</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>673</v>
+        <v>677</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>674</v>
+        <v>678</v>
       </c>
     </row>
     <row r="4" ht="127.5" spans="1:3">
       <c r="A4" s="11"/>
       <c r="B4" s="12" t="s">
-        <v>675</v>
+        <v>679</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>676</v>
+        <v>680</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="11"/>
       <c r="B5" t="s">
-        <v>677</v>
+        <v>681</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="11"/>
       <c r="B6" t="s">
-        <v>678</v>
+        <v>682</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="11"/>
       <c r="B7" t="s">
-        <v>679</v>
+        <v>683</v>
       </c>
     </row>
     <row r="8" ht="76.5" spans="1:3">
       <c r="A8" s="11"/>
       <c r="B8" s="13" t="s">
-        <v>680</v>
+        <v>684</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>681</v>
+        <v>685</v>
       </c>
     </row>
     <row r="9" ht="102" spans="1:3">
       <c r="A9" s="11"/>
       <c r="B9" s="13"/>
       <c r="C9" s="5" t="s">
-        <v>682</v>
+        <v>686</v>
       </c>
     </row>
     <row r="10" ht="76.5" spans="1:3">
       <c r="A10" s="11"/>
       <c r="B10" s="13"/>
       <c r="C10" s="5" t="s">
-        <v>683</v>
+        <v>687</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="11"/>
       <c r="B11" s="13"/>
       <c r="C11" t="s">
-        <v>684</v>
+        <v>688</v>
       </c>
     </row>
     <row r="12" ht="63.75" spans="1:3">
       <c r="A12" s="11"/>
       <c r="B12" s="13"/>
       <c r="C12" s="2" t="s">
-        <v>685</v>
+        <v>689</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="11"/>
       <c r="B13" t="s">
-        <v>686</v>
+        <v>690</v>
       </c>
     </row>
     <row r="14" ht="191.25" spans="1:3">
       <c r="A14" s="11"/>
       <c r="B14" s="14" t="s">
-        <v>687</v>
+        <v>691</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>688</v>
+        <v>692</v>
       </c>
     </row>
     <row r="15" ht="153" spans="1:3">
       <c r="A15" s="11"/>
       <c r="B15" s="14"/>
       <c r="C15" s="15" t="s">
-        <v>689</v>
+        <v>693</v>
       </c>
     </row>
     <row r="16" ht="102" spans="1:3">
       <c r="A16" s="11"/>
       <c r="B16" s="14"/>
       <c r="C16" s="15" t="s">
-        <v>690</v>
+        <v>694</v>
       </c>
     </row>
     <row r="17" ht="38.25" spans="1:3">
       <c r="A17" s="11"/>
       <c r="B17" s="14"/>
       <c r="C17" s="15" t="s">
-        <v>691</v>
+        <v>695</v>
       </c>
     </row>
     <row r="18" ht="76.5" spans="1:3">
       <c r="A18" s="11"/>
       <c r="B18" s="14"/>
       <c r="C18" s="5" t="s">
-        <v>692</v>
+        <v>696</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -12485,13 +12576,13 @@
     <row r="20" spans="1:2">
       <c r="A20" s="11"/>
       <c r="B20" s="17" t="s">
-        <v>693</v>
+        <v>697</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="11"/>
       <c r="B21" t="s">
-        <v>694</v>
+        <v>698</v>
       </c>
     </row>
     <row r="22" spans="1:1">
@@ -12502,40 +12593,40 @@
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="11" t="s">
-        <v>695</v>
+        <v>699</v>
       </c>
       <c r="B24" t="s">
-        <v>696</v>
+        <v>700</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="11"/>
       <c r="B25" t="s">
-        <v>697</v>
+        <v>701</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" s="11"/>
       <c r="B26" t="s">
-        <v>698</v>
+        <v>702</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" s="11"/>
       <c r="B27" t="s">
-        <v>699</v>
+        <v>703</v>
       </c>
     </row>
     <row r="28" ht="51" spans="1:2">
       <c r="A28" s="11"/>
       <c r="B28" s="2" t="s">
-        <v>700</v>
+        <v>704</v>
       </c>
     </row>
     <row r="29" ht="127.5" spans="1:2">
       <c r="A29" s="11"/>
       <c r="B29" s="2" t="s">
-        <v>701</v>
+        <v>705</v>
       </c>
     </row>
     <row r="30" spans="1:1">
@@ -12543,41 +12634,41 @@
     </row>
     <row r="31" ht="102" spans="1:6">
       <c r="A31" s="11" t="s">
-        <v>702</v>
+        <v>706</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>703</v>
+        <v>707</v>
       </c>
       <c r="F31" s="19"/>
     </row>
     <row r="32" ht="51" spans="1:2">
       <c r="A32" s="11"/>
       <c r="B32" s="2" t="s">
-        <v>704</v>
+        <v>708</v>
       </c>
     </row>
     <row r="33" ht="25.5" spans="1:2">
       <c r="A33" s="11"/>
       <c r="B33" s="2" t="s">
-        <v>705</v>
+        <v>709</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" s="11"/>
       <c r="B34" s="2" t="s">
-        <v>706</v>
+        <v>710</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" s="11"/>
       <c r="B35" s="2" t="s">
-        <v>707</v>
+        <v>711</v>
       </c>
     </row>
     <row r="36" ht="114.75" spans="1:3">
       <c r="A36" s="11"/>
       <c r="B36" s="2" t="s">
-        <v>708</v>
+        <v>712</v>
       </c>
       <c r="C36" s="2"/>
     </row>
@@ -12630,7 +12721,7 @@
       <c r="A3" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="B3" s="85" t="s">
+      <c r="B3" s="83" t="s">
         <v>45</v>
       </c>
     </row>
@@ -12638,7 +12729,7 @@
       <c r="A4" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="B4" s="84" t="s">
+      <c r="B4" s="82" t="s">
         <v>47</v>
       </c>
     </row>
@@ -12646,7 +12737,7 @@
       <c r="A5" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="B5" s="85" t="s">
+      <c r="B5" s="83" t="s">
         <v>49</v>
       </c>
     </row>
@@ -12654,7 +12745,7 @@
       <c r="A6" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="B6" s="85" t="s">
+      <c r="B6" s="83" t="s">
         <v>51</v>
       </c>
     </row>
@@ -12667,10 +12758,10 @@
       <c r="A8" s="6"/>
     </row>
     <row r="9" ht="25.5" spans="1:2">
-      <c r="A9" s="86" t="s">
+      <c r="A9" s="84" t="s">
         <v>53</v>
       </c>
-      <c r="B9" s="85" t="s">
+      <c r="B9" s="83" t="s">
         <v>54</v>
       </c>
     </row>
@@ -12686,36 +12777,36 @@
       </c>
     </row>
     <row r="13" spans="1:1">
-      <c r="A13" s="69" t="s">
+      <c r="A13" s="67" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="14" spans="1:2">
-      <c r="A14" s="70" t="s">
+      <c r="A14" s="68" t="s">
         <v>57</v>
       </c>
-      <c r="B14" s="71" t="s">
+      <c r="B14" s="69" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:2">
-      <c r="A15" s="69" t="s">
+      <c r="A15" s="67" t="s">
         <v>59</v>
       </c>
-      <c r="B15" s="72" t="s">
+      <c r="B15" s="70" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="16" ht="48" spans="1:2">
-      <c r="A16" s="70" t="s">
+      <c r="A16" s="68" t="s">
         <v>61</v>
       </c>
-      <c r="B16" s="73" t="s">
+      <c r="B16" s="71" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="17" spans="1:2">
-      <c r="A17" s="69" t="s">
+      <c r="A17" s="67" t="s">
         <v>63</v>
       </c>
       <c r="B17" s="41" t="s">
@@ -12723,7 +12814,7 @@
       </c>
     </row>
     <row r="18" spans="1:2">
-      <c r="A18" s="70" t="s">
+      <c r="A18" s="68" t="s">
         <v>65</v>
       </c>
       <c r="B18" s="40" t="s">
@@ -12731,7 +12822,7 @@
       </c>
     </row>
     <row r="19" spans="1:2">
-      <c r="A19" s="69" t="s">
+      <c r="A19" s="67" t="s">
         <v>67</v>
       </c>
       <c r="B19" s="41"/>
@@ -12988,13 +13079,13 @@
     </row>
     <row r="59" ht="76.5" spans="1:2">
       <c r="A59" s="52"/>
-      <c r="B59" s="74" t="s">
+      <c r="B59" s="72" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="60" ht="318.75" spans="1:2">
       <c r="A60" s="52"/>
-      <c r="B60" s="75" t="s">
+      <c r="B60" s="73" t="s">
         <v>120</v>
       </c>
     </row>
@@ -13023,7 +13114,7 @@
       </c>
     </row>
     <row r="64" ht="116.25" spans="1:2">
-      <c r="A64" s="76" t="s">
+      <c r="A64" s="74" t="s">
         <v>127</v>
       </c>
       <c r="B64" s="8" t="s">
@@ -13031,7 +13122,7 @@
       </c>
     </row>
     <row r="65" ht="129" spans="1:2">
-      <c r="A65" s="76" t="s">
+      <c r="A65" s="74" t="s">
         <v>129</v>
       </c>
       <c r="B65" s="8" t="s">
@@ -13039,16 +13130,16 @@
       </c>
     </row>
     <row r="66" ht="14.25" spans="1:2">
-      <c r="A66" s="76"/>
-      <c r="B66" s="77" t="s">
+      <c r="A66" s="74"/>
+      <c r="B66" s="75" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="67" ht="13.5" spans="1:2">
-      <c r="A67" s="78" t="s">
+      <c r="A67" s="76" t="s">
         <v>132</v>
       </c>
-      <c r="B67" s="79" t="s">
+      <c r="B67" s="77" t="s">
         <v>133</v>
       </c>
     </row>
@@ -13060,13 +13151,13 @@
     </row>
     <row r="69" ht="25.5" spans="1:2">
       <c r="A69" s="53"/>
-      <c r="B69" s="75" t="s">
+      <c r="B69" s="73" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="70" spans="1:2">
       <c r="A70" s="53"/>
-      <c r="B70" s="79" t="s">
+      <c r="B70" s="77" t="s">
         <v>136</v>
       </c>
     </row>
@@ -13080,7 +13171,7 @@
     </row>
     <row r="72" spans="1:2">
       <c r="A72" s="6"/>
-      <c r="B72" s="77" t="s">
+      <c r="B72" s="75" t="s">
         <v>139</v>
       </c>
     </row>
@@ -13132,7 +13223,7 @@
     </row>
     <row r="80" spans="1:2">
       <c r="A80" s="6"/>
-      <c r="B80" s="77" t="s">
+      <c r="B80" s="75" t="s">
         <v>149</v>
       </c>
     </row>
@@ -13150,90 +13241,90 @@
       <c r="A83" s="53" t="s">
         <v>152</v>
       </c>
-      <c r="B83" s="80" t="s">
+      <c r="B83" s="78" t="s">
         <v>153</v>
       </c>
-      <c r="C83" s="81" t="s">
+      <c r="C83" s="79" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="84" ht="14.25" spans="1:3">
       <c r="A84" s="53"/>
-      <c r="B84" s="80"/>
-      <c r="C84" s="81" t="s">
+      <c r="B84" s="78"/>
+      <c r="C84" s="79" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="85" ht="14.25" spans="1:3">
       <c r="A85" s="53"/>
-      <c r="B85" s="80" t="s">
+      <c r="B85" s="78" t="s">
         <v>156</v>
       </c>
-      <c r="C85" s="81" t="s">
+      <c r="C85" s="79" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="86" ht="14.25" spans="1:3">
       <c r="A86" s="53"/>
-      <c r="B86" s="80"/>
-      <c r="C86" s="81" t="s">
+      <c r="B86" s="78"/>
+      <c r="C86" s="79" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="87" ht="14.25" spans="1:3">
       <c r="A87" s="53"/>
-      <c r="B87" s="80" t="s">
+      <c r="B87" s="78" t="s">
         <v>158</v>
       </c>
-      <c r="C87" s="81" t="s">
+      <c r="C87" s="79" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="88" ht="14.25" spans="1:3">
       <c r="A88" s="53"/>
-      <c r="B88" s="80" t="s">
+      <c r="B88" s="78" t="s">
         <v>160</v>
       </c>
-      <c r="C88" s="81" t="s">
+      <c r="C88" s="79" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="89" ht="14.25" spans="1:3">
       <c r="A89" s="53"/>
-      <c r="B89" s="80"/>
-      <c r="C89" s="81" t="s">
+      <c r="B89" s="78"/>
+      <c r="C89" s="79" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="90" ht="14.25" spans="1:3">
       <c r="A90" s="53"/>
-      <c r="B90" s="80" t="s">
+      <c r="B90" s="78" t="s">
         <v>162</v>
       </c>
-      <c r="C90" s="81"/>
+      <c r="C90" s="79"/>
     </row>
     <row r="91" ht="14.25" spans="1:3">
       <c r="A91" s="53"/>
-      <c r="B91" s="80" t="s">
+      <c r="B91" s="78" t="s">
         <v>163</v>
       </c>
-      <c r="C91" s="81" t="s">
+      <c r="C91" s="79" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="92" ht="14.25" spans="1:3">
       <c r="A92" s="53"/>
-      <c r="B92" s="80"/>
-      <c r="C92" s="81" t="s">
+      <c r="B92" s="78"/>
+      <c r="C92" s="79" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="93" ht="14.25" spans="1:3">
       <c r="A93" s="53"/>
-      <c r="B93" s="80" t="s">
+      <c r="B93" s="78" t="s">
         <v>166</v>
       </c>
-      <c r="C93" s="81" t="s">
+      <c r="C93" s="79" t="s">
         <v>167</v>
       </c>
     </row>
@@ -13315,26 +13406,26 @@
   <sheetData>
     <row r="1" ht="153" spans="1:2">
       <c r="A1" s="7" t="s">
-        <v>709</v>
+        <v>713</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>710</v>
+        <v>714</v>
       </c>
     </row>
     <row r="2" ht="76.5" spans="1:2">
       <c r="A2" s="8" t="s">
-        <v>711</v>
+        <v>715</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>712</v>
+        <v>716</v>
       </c>
     </row>
     <row r="3" ht="153" spans="1:2">
       <c r="A3" s="8" t="s">
-        <v>713</v>
+        <v>717</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>714</v>
+        <v>718</v>
       </c>
     </row>
   </sheetData>
@@ -13376,96 +13467,96 @@
   <sheetData>
     <row r="2" ht="51" spans="1:2">
       <c r="A2" t="s">
-        <v>715</v>
+        <v>719</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>716</v>
+        <v>720</v>
       </c>
     </row>
     <row r="3" ht="127.5" spans="1:2">
       <c r="A3" t="s">
-        <v>717</v>
+        <v>721</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>718</v>
+        <v>722</v>
       </c>
     </row>
     <row r="4" ht="114.75" spans="1:2">
       <c r="A4" t="s">
-        <v>719</v>
+        <v>723</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>720</v>
+        <v>724</v>
       </c>
     </row>
     <row r="5" ht="63.75" spans="1:2">
       <c r="A5" t="s">
-        <v>514</v>
+        <v>518</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>721</v>
+        <v>725</v>
       </c>
     </row>
     <row r="6" ht="38.25" spans="1:2">
       <c r="A6" t="s">
-        <v>722</v>
+        <v>726</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>723</v>
+        <v>727</v>
       </c>
     </row>
     <row r="7" ht="38.25" spans="1:2">
       <c r="A7" t="s">
-        <v>724</v>
+        <v>728</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>725</v>
+        <v>729</v>
       </c>
     </row>
     <row r="8" ht="63.75" spans="1:2">
       <c r="A8" t="s">
-        <v>726</v>
+        <v>730</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>727</v>
+        <v>731</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="6" t="s">
-        <v>728</v>
+        <v>732</v>
       </c>
       <c r="B9" t="s">
-        <v>729</v>
+        <v>733</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="6"/>
       <c r="B10" t="s">
-        <v>730</v>
+        <v>734</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="6"/>
       <c r="B11" t="s">
-        <v>731</v>
+        <v>735</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="6"/>
       <c r="B12" t="s">
-        <v>732</v>
+        <v>736</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="6"/>
       <c r="B13" t="s">
-        <v>733</v>
+        <v>737</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="6"/>
       <c r="B14" t="s">
-        <v>734</v>
+        <v>738</v>
       </c>
     </row>
   </sheetData>
@@ -13495,110 +13586,110 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>735</v>
+        <v>739</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>736</v>
+        <v>740</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>737</v>
+        <v>741</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>738</v>
+        <v>742</v>
       </c>
     </row>
     <row r="4" ht="63.75" spans="1:2">
       <c r="A4" t="s">
-        <v>739</v>
+        <v>743</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>740</v>
+        <v>744</v>
       </c>
     </row>
     <row r="6" ht="51" spans="1:2">
       <c r="A6" t="s">
-        <v>741</v>
+        <v>745</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>742</v>
+        <v>746</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" t="s">
-        <v>743</v>
+        <v>747</v>
       </c>
     </row>
     <row r="10" ht="38.25" spans="1:2">
       <c r="A10" t="s">
-        <v>744</v>
+        <v>748</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>745</v>
+        <v>749</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" t="s">
-        <v>746</v>
+        <v>750</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" t="s">
-        <v>747</v>
+        <v>751</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16" t="s">
-        <v>748</v>
+        <v>752</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" t="s">
-        <v>749</v>
+        <v>753</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" t="s">
-        <v>750</v>
+        <v>754</v>
       </c>
     </row>
     <row r="25" spans="1:1">
       <c r="A25" s="3" t="s">
-        <v>751</v>
+        <v>755</v>
       </c>
     </row>
     <row r="27" ht="89.25" spans="1:2">
       <c r="A27" s="4" t="s">
-        <v>752</v>
+        <v>756</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>753</v>
+        <v>757</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" s="4"/>
       <c r="B28" t="s">
-        <v>754</v>
+        <v>758</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" s="4"/>
       <c r="B29" t="s">
-        <v>755</v>
+        <v>759</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" s="4"/>
       <c r="B30" t="s">
-        <v>756</v>
+        <v>760</v>
       </c>
     </row>
     <row r="31" spans="2:2">
       <c r="B31" t="s">
-        <v>748</v>
+        <v>752</v>
       </c>
     </row>
   </sheetData>
@@ -13670,7 +13761,7 @@
       </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="62" t="s">
+      <c r="A4" s="60" t="s">
         <v>175</v>
       </c>
       <c r="B4" s="35" t="s">
@@ -13681,43 +13772,43 @@
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="63"/>
+      <c r="A5" s="61"/>
       <c r="B5" s="38" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="63"/>
+      <c r="A6" s="61"/>
       <c r="B6" s="35" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="63"/>
+      <c r="A7" s="61"/>
       <c r="B7" s="38" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" s="63"/>
+      <c r="A8" s="61"/>
       <c r="B8" s="35" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" s="63"/>
+      <c r="A9" s="61"/>
       <c r="B9" s="38" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" s="63"/>
+      <c r="A10" s="61"/>
       <c r="B10" s="35" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" s="64"/>
+      <c r="A11" s="62"/>
       <c r="B11" s="38" t="s">
         <v>184</v>
       </c>
@@ -13781,7 +13872,7 @@
       </c>
     </row>
     <row r="23" ht="204" spans="1:2">
-      <c r="A23" s="65" t="s">
+      <c r="A23" s="63" t="s">
         <v>194</v>
       </c>
       <c r="B23" s="2" t="s">
@@ -13851,7 +13942,7 @@
       <c r="B31" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="C31" s="66" t="s">
+      <c r="C31" s="64" t="s">
         <v>212</v>
       </c>
     </row>
@@ -13864,7 +13955,7 @@
     </row>
     <row r="33" ht="114.75" spans="1:3">
       <c r="A33" s="6"/>
-      <c r="B33" s="67" t="s">
+      <c r="B33" s="65" t="s">
         <v>214</v>
       </c>
       <c r="C33" s="34"/>
@@ -13889,10 +13980,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C119"/>
+  <dimension ref="A1:C123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A114" workbookViewId="0">
-      <selection activeCell="B118" sqref="B118"/>
+    <sheetView tabSelected="1" topLeftCell="A99" workbookViewId="0">
+      <selection activeCell="B102" sqref="B102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" outlineLevelCol="2"/>
@@ -13919,7 +14010,7 @@
       <c r="A3" s="28" t="s">
         <v>218</v>
       </c>
-      <c r="B3" s="85" t="s">
+      <c r="B3" s="83" t="s">
         <v>219</v>
       </c>
     </row>
@@ -14351,8 +14442,8 @@
         <v>291</v>
       </c>
     </row>
-    <row r="79" ht="114.75" spans="1:3">
-      <c r="A79" s="6" t="s">
+    <row r="79" ht="216.75" spans="1:3">
+      <c r="A79" s="18" t="s">
         <v>292</v>
       </c>
       <c r="B79" s="5" t="s">
@@ -14545,25 +14636,51 @@
       </c>
     </row>
     <row r="117" ht="76.5" spans="1:2">
-      <c r="A117" s="59" t="s">
+      <c r="A117" s="6" t="s">
         <v>328</v>
       </c>
-      <c r="B117" s="60" t="s">
+      <c r="B117" s="15" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="118" ht="76.5" spans="2:2">
-      <c r="B118" s="60" t="s">
+    <row r="118" ht="76.5" spans="1:2">
+      <c r="A118" s="6"/>
+      <c r="B118" s="15" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="119" ht="63.75" spans="2:2">
-      <c r="B119" s="61" t="s">
+    <row r="119" spans="1:2">
+      <c r="A119" s="6"/>
+      <c r="B119" s="13" t="s">
         <v>331</v>
       </c>
     </row>
+    <row r="120" ht="63.75" spans="1:2">
+      <c r="A120" s="6"/>
+      <c r="B120" s="2" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="121" ht="25.5" spans="1:2">
+      <c r="A121" s="6"/>
+      <c r="B121" s="2" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="122" ht="25.5" spans="1:2">
+      <c r="A122" s="6"/>
+      <c r="B122" s="59" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="123" ht="25.5" spans="1:2">
+      <c r="A123" s="6"/>
+      <c r="B123" s="59" t="s">
+        <v>335</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="13">
+  <mergeCells count="14">
     <mergeCell ref="A38:A42"/>
     <mergeCell ref="A50:A52"/>
     <mergeCell ref="A56:A59"/>
@@ -14576,6 +14693,7 @@
     <mergeCell ref="A102:A105"/>
     <mergeCell ref="A108:A111"/>
     <mergeCell ref="A113:A115"/>
+    <mergeCell ref="A117:A123"/>
     <mergeCell ref="B56:B59"/>
   </mergeCells>
   <hyperlinks>
@@ -14610,114 +14728,114 @@
   <sheetData>
     <row r="1" ht="51" spans="1:2">
       <c r="A1" s="7" t="s">
-        <v>332</v>
+        <v>336</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>333</v>
+        <v>337</v>
       </c>
     </row>
     <row r="2" ht="63.75" spans="1:2">
       <c r="A2" s="8" t="s">
-        <v>334</v>
+        <v>338</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>335</v>
+        <v>339</v>
       </c>
     </row>
     <row r="3" ht="25.5" spans="1:2">
       <c r="A3" s="47" t="s">
-        <v>336</v>
+        <v>340</v>
       </c>
       <c r="B3" s="48" t="s">
-        <v>337</v>
+        <v>341</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="47" t="s">
-        <v>338</v>
+        <v>342</v>
       </c>
       <c r="B4" s="48" t="s">
-        <v>339</v>
+        <v>343</v>
       </c>
     </row>
     <row r="5" ht="64.5" customHeight="1" spans="1:2">
-      <c r="A5" s="87" t="s">
-        <v>340</v>
+      <c r="A5" s="85" t="s">
+        <v>344</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>341</v>
+        <v>345</v>
       </c>
     </row>
     <row r="6" ht="52.5" customHeight="1" spans="1:1">
       <c r="A6" s="7" t="s">
-        <v>342</v>
+        <v>346</v>
       </c>
     </row>
     <row r="7" ht="82.5" customHeight="1" spans="1:1">
       <c r="A7" s="8" t="s">
-        <v>343</v>
+        <v>347</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="49" t="s">
-        <v>344</v>
+        <v>348</v>
       </c>
       <c r="B8" s="38" t="s">
-        <v>345</v>
+        <v>349</v>
       </c>
       <c r="C8" s="50" t="s">
-        <v>346</v>
+        <v>350</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="39"/>
       <c r="B9" s="35" t="s">
-        <v>347</v>
+        <v>351</v>
       </c>
       <c r="C9" s="39"/>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="39"/>
       <c r="B10" s="38" t="s">
-        <v>348</v>
+        <v>352</v>
       </c>
       <c r="C10" s="39"/>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="39"/>
       <c r="B11" s="35" t="s">
-        <v>349</v>
+        <v>353</v>
       </c>
       <c r="C11" s="39"/>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="42"/>
       <c r="B12" s="38" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="C12" s="42"/>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="7" t="s">
-        <v>351</v>
+        <v>355</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>352</v>
+        <v>356</v>
       </c>
     </row>
     <row r="16" spans="2:2">
       <c r="B16" s="8" t="s">
-        <v>353</v>
+        <v>357</v>
       </c>
     </row>
     <row r="17" spans="2:2">
       <c r="B17" s="8" t="s">
-        <v>354</v>
+        <v>358</v>
       </c>
     </row>
     <row r="18" spans="2:2">
       <c r="B18" s="8" t="s">
-        <v>355</v>
+        <v>359</v>
       </c>
     </row>
     <row r="20" ht="293.25" spans="1:2">
@@ -14725,185 +14843,185 @@
         <v>23</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>356</v>
+        <v>360</v>
       </c>
     </row>
     <row r="22" ht="89.25" spans="1:3">
       <c r="A22" s="7" t="s">
-        <v>357</v>
+        <v>361</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>358</v>
+        <v>362</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>359</v>
+        <v>363</v>
       </c>
     </row>
     <row r="24" ht="153" spans="1:3">
       <c r="A24" s="7" t="s">
-        <v>360</v>
+        <v>364</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>361</v>
+        <v>365</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>359</v>
+        <v>363</v>
       </c>
     </row>
     <row r="26" ht="63.75" spans="1:11">
       <c r="A26" s="7" t="s">
-        <v>362</v>
+        <v>366</v>
       </c>
       <c r="B26" s="8" t="s">
+        <v>367</v>
+      </c>
+      <c r="C26" s="1" t="s">
         <v>363</v>
       </c>
-      <c r="C26" s="1" t="s">
-        <v>359</v>
-      </c>
       <c r="K26" s="1" t="s">
-        <v>364</v>
+        <v>368</v>
       </c>
     </row>
     <row r="28" spans="2:3">
       <c r="B28" s="29" t="s">
-        <v>365</v>
+        <v>369</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>366</v>
+        <v>370</v>
       </c>
     </row>
     <row r="29" ht="25.5" spans="1:2">
       <c r="A29" s="7" t="s">
-        <v>367</v>
+        <v>371</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>368</v>
+        <v>372</v>
       </c>
     </row>
     <row r="31" ht="102" spans="1:2">
       <c r="A31" s="7" t="s">
-        <v>369</v>
+        <v>373</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>370</v>
+        <v>374</v>
       </c>
     </row>
     <row r="32" ht="25.5" spans="1:2">
       <c r="A32" s="7" t="s">
-        <v>371</v>
+        <v>375</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>372</v>
+        <v>376</v>
       </c>
     </row>
     <row r="33" ht="127.5" spans="1:2">
       <c r="A33" s="7" t="s">
-        <v>373</v>
+        <v>377</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>374</v>
+        <v>378</v>
       </c>
     </row>
     <row r="34" ht="229.5" spans="1:3">
       <c r="A34" s="46" t="s">
-        <v>375</v>
+        <v>379</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>376</v>
+        <v>380</v>
       </c>
       <c r="C34" s="51" t="s">
-        <v>377</v>
+        <v>381</v>
       </c>
     </row>
     <row r="36" ht="38.25" spans="1:2">
       <c r="A36" s="7" t="s">
-        <v>378</v>
+        <v>382</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>379</v>
+        <v>383</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" s="7" t="s">
-        <v>380</v>
+        <v>384</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>381</v>
+        <v>385</v>
       </c>
     </row>
     <row r="38" spans="1:1">
       <c r="A38" s="7" t="s">
-        <v>382</v>
+        <v>386</v>
       </c>
     </row>
     <row r="39" spans="1:1">
       <c r="A39" s="7" t="s">
-        <v>383</v>
+        <v>387</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" s="7" t="s">
-        <v>384</v>
+        <v>388</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>385</v>
+        <v>389</v>
       </c>
     </row>
     <row r="41" ht="165.75" spans="1:3">
       <c r="A41" s="7" t="s">
-        <v>386</v>
+        <v>390</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>387</v>
+        <v>391</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>388</v>
+        <v>392</v>
       </c>
     </row>
     <row r="42" spans="1:3">
       <c r="A42" s="7" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>388</v>
+        <v>392</v>
       </c>
     </row>
     <row r="43" ht="140.25" spans="1:3">
       <c r="A43" s="52" t="s">
-        <v>390</v>
+        <v>394</v>
       </c>
       <c r="B43" s="28" t="s">
-        <v>391</v>
+        <v>395</v>
       </c>
       <c r="C43" s="15" t="s">
-        <v>392</v>
+        <v>396</v>
       </c>
     </row>
     <row r="44" ht="102" spans="1:3">
       <c r="A44" s="52"/>
       <c r="B44" s="28" t="s">
-        <v>390</v>
+        <v>394</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
     </row>
     <row r="45" ht="140.25" spans="1:3">
       <c r="A45" s="52"/>
       <c r="B45" s="28" t="s">
-        <v>394</v>
+        <v>398</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>395</v>
+        <v>399</v>
       </c>
     </row>
     <row r="46" ht="25.5" spans="1:3">
       <c r="A46" s="52"/>
       <c r="B46" s="28" t="s">
-        <v>396</v>
+        <v>400</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>397</v>
+        <v>401</v>
       </c>
     </row>
   </sheetData>
@@ -14946,46 +15064,46 @@
   <sheetData>
     <row r="1" ht="25.5" spans="1:2">
       <c r="A1" s="43" t="s">
-        <v>398</v>
+        <v>402</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>399</v>
+        <v>403</v>
       </c>
     </row>
     <row r="2" ht="76.5" spans="1:2">
       <c r="A2" s="44"/>
       <c r="B2" s="15" t="s">
-        <v>400</v>
+        <v>404</v>
       </c>
     </row>
     <row r="3" ht="63.75" spans="1:2">
       <c r="A3" s="44"/>
       <c r="B3" s="15" t="s">
-        <v>401</v>
+        <v>405</v>
       </c>
     </row>
     <row r="4" ht="63.75" spans="1:2">
       <c r="A4" s="44"/>
       <c r="B4" s="15" t="s">
-        <v>402</v>
+        <v>406</v>
       </c>
     </row>
     <row r="5" ht="25.5" spans="1:2">
       <c r="A5" s="44"/>
       <c r="B5" s="15" t="s">
-        <v>403</v>
+        <v>407</v>
       </c>
     </row>
     <row r="6" ht="114.75" spans="1:2">
       <c r="A6" s="44"/>
       <c r="B6" s="2" t="s">
-        <v>404</v>
+        <v>408</v>
       </c>
     </row>
     <row r="7" ht="17.25" spans="1:2">
       <c r="A7" s="44"/>
       <c r="B7" s="45" t="s">
-        <v>405</v>
+        <v>409</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -15075,22 +15193,22 @@
     </row>
     <row r="36" ht="38.25" spans="1:2">
       <c r="A36" s="44" t="s">
-        <v>406</v>
+        <v>410</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>407</v>
+        <v>411</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" s="44"/>
       <c r="B37" s="17" t="s">
-        <v>408</v>
+        <v>412</v>
       </c>
     </row>
     <row r="38" ht="17.25" spans="1:2">
       <c r="A38" s="44"/>
       <c r="B38" s="45" t="s">
-        <v>405</v>
+        <v>409</v>
       </c>
     </row>
     <row r="39" spans="1:1">
@@ -15209,88 +15327,88 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="35" t="s">
-        <v>409</v>
+        <v>413</v>
       </c>
       <c r="B1" s="36" t="s">
-        <v>410</v>
+        <v>414</v>
       </c>
       <c r="C1" s="37" t="s">
-        <v>411</v>
+        <v>415</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="38" t="s">
-        <v>412</v>
+        <v>416</v>
       </c>
       <c r="B2" s="39"/>
       <c r="C2" s="40"/>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="35" t="s">
-        <v>413</v>
+        <v>417</v>
       </c>
       <c r="B3" s="39"/>
       <c r="C3" s="41"/>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="38" t="s">
-        <v>414</v>
+        <v>418</v>
       </c>
       <c r="B4" s="39"/>
       <c r="C4" s="40"/>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="35" t="s">
-        <v>415</v>
+        <v>419</v>
       </c>
       <c r="B5" s="39"/>
       <c r="C5" s="41"/>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="38" t="s">
-        <v>416</v>
+        <v>420</v>
       </c>
       <c r="B6" s="39"/>
       <c r="C6" s="40"/>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="35" t="s">
-        <v>417</v>
+        <v>421</v>
       </c>
       <c r="B7" s="42"/>
       <c r="C7" s="41"/>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>415</v>
+        <v>419</v>
       </c>
       <c r="B12" t="s">
-        <v>418</v>
+        <v>422</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" t="s">
-        <v>419</v>
+        <v>423</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16" t="s">
-        <v>420</v>
+        <v>424</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" t="s">
-        <v>421</v>
+        <v>425</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" t="s">
-        <v>422</v>
+        <v>426</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" t="s">
-        <v>423</v>
+        <v>427</v>
       </c>
     </row>
   </sheetData>
@@ -15324,92 +15442,92 @@
   <sheetData>
     <row r="2" ht="140.25" spans="1:2">
       <c r="A2" t="s">
-        <v>424</v>
+        <v>428</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>425</v>
+        <v>429</v>
       </c>
     </row>
     <row r="3" ht="25.5" spans="1:2">
       <c r="A3" t="s">
-        <v>426</v>
+        <v>430</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>427</v>
+        <v>431</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>428</v>
+        <v>432</v>
       </c>
       <c r="B4" t="s">
-        <v>429</v>
+        <v>433</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>430</v>
+        <v>434</v>
       </c>
       <c r="B6" t="s">
-        <v>431</v>
+        <v>435</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>432</v>
+        <v>436</v>
       </c>
       <c r="B7" t="s">
-        <v>433</v>
+        <v>437</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>434</v>
+        <v>438</v>
       </c>
       <c r="B8" t="s">
-        <v>435</v>
+        <v>439</v>
       </c>
     </row>
     <row r="9" ht="45" customHeight="1" spans="1:2">
       <c r="A9" t="s">
-        <v>436</v>
+        <v>440</v>
       </c>
       <c r="B9" t="s">
-        <v>437</v>
+        <v>441</v>
       </c>
     </row>
     <row r="10" ht="63.75" spans="1:2">
       <c r="A10" t="s">
-        <v>438</v>
+        <v>442</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>439</v>
+        <v>443</v>
       </c>
     </row>
     <row r="11" ht="63.75" spans="1:4">
       <c r="A11" s="34" t="s">
-        <v>440</v>
+        <v>444</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>441</v>
+        <v>445</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>442</v>
+        <v>446</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>443</v>
+        <v>447</v>
       </c>
     </row>
     <row r="12" ht="76.5" spans="1:4">
       <c r="A12" s="34"/>
       <c r="B12" s="2" t="s">
-        <v>444</v>
+        <v>448</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>445</v>
+        <v>449</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>446</v>
+        <v>450</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[feat][system-design][Update system design sheet]
</commit_message>
<xml_diff>
--- a/Doc/Documents.xlsx
+++ b/Doc/Documents.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WorkSpace\MyProject\My-Documents\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EE24EF3-1F04-4162-BC1E-3A5E15C843AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CB410A0-D1F4-41A9-8EC9-1763450CCA7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" firstSheet="7" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
     <sheet name="6.DesignPattern" sheetId="10" r:id="rId8"/>
     <sheet name="7.OOP - AOP" sheetId="15" r:id="rId9"/>
     <sheet name="8.Annotations" sheetId="21" r:id="rId10"/>
-    <sheet name="9.System Design" sheetId="22" r:id="rId11"/>
+    <sheet name="9.Architechture" sheetId="22" r:id="rId11"/>
     <sheet name="10.Microservice" sheetId="3" r:id="rId12"/>
     <sheet name="11.Cache" sheetId="11" r:id="rId13"/>
     <sheet name="12.Git" sheetId="7" r:id="rId14"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="768" uniqueCount="751">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="750" uniqueCount="735">
   <si>
     <t>Kiến Trúc về Microservice</t>
   </si>
@@ -6194,55 +6194,10 @@
     <t>@ConditionalOnResource</t>
   </si>
   <si>
-    <t>Database</t>
-  </si>
-  <si>
-    <t>Microservices vs Moniliths</t>
-  </si>
-  <si>
-    <t>API Design</t>
-  </si>
-  <si>
-    <t>Data Partitioning</t>
-  </si>
-  <si>
     <t>Caching</t>
   </si>
   <si>
-    <t>Rate Limiting</t>
-  </si>
-  <si>
-    <t>Message Queues</t>
-  </si>
-  <si>
-    <t>Monitoring and Logging</t>
-  </si>
-  <si>
-    <t>Security</t>
-  </si>
-  <si>
-    <t>Connecting Protocols</t>
-  </si>
-  <si>
-    <t>Scalability</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Consistency </t>
-  </si>
-  <si>
-    <t>Availabiblity</t>
-  </si>
-  <si>
     <t>Concurrency</t>
-  </si>
-  <si>
-    <t>Reliability</t>
-  </si>
-  <si>
-    <t>Course</t>
-  </si>
-  <si>
-    <t>https://www.geeksforgeeks.org/system-design-tutorial/?ref=lbp</t>
   </si>
   <si>
     <t>Domain Driven Design</t>
@@ -9260,27 +9215,17 @@
   <si>
     <t>SYSTEM DESIGN</t>
   </si>
-  <si>
-    <t>Concepts</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="24">
+  <fonts count="26">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -9434,7 +9379,29 @@
     </font>
     <font>
       <b/>
-      <sz val="12"/>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -9442,9 +9409,9 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="8">
@@ -9578,14 +9545,14 @@
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="92">
+  <cellXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="4"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -9599,57 +9566,54 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="3"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="4" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="4" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="4" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="4" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="2" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -9661,7 +9625,7 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="4" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="4" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -9670,65 +9634,65 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="2" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="5" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="5" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="4" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="4" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
@@ -9740,8 +9704,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -9749,10 +9723,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="5" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -9761,19 +9738,16 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="5" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="4" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="4" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -9782,53 +9756,59 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="4" applyFont="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="4" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -10467,7 +10447,7 @@
       <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="56" t="s">
+      <c r="C1" s="55" t="s">
         <v>1</v>
       </c>
     </row>
@@ -10478,7 +10458,7 @@
       <c r="B2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="56" t="s">
+      <c r="C2" s="55" t="s">
         <v>3</v>
       </c>
     </row>
@@ -10486,10 +10466,10 @@
       <c r="A3" s="5">
         <v>3</v>
       </c>
-      <c r="B3" s="54" t="s">
+      <c r="B3" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="56" t="s">
+      <c r="C3" s="55" t="s">
         <v>5</v>
       </c>
     </row>
@@ -10500,7 +10480,7 @@
       <c r="B4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="57" t="s">
+      <c r="C4" s="56" t="s">
         <v>7</v>
       </c>
     </row>
@@ -10522,7 +10502,7 @@
       <c r="B6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="57" t="s">
+      <c r="C6" s="56" t="s">
         <v>11</v>
       </c>
     </row>
@@ -10533,7 +10513,7 @@
       <c r="B7" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="41" t="s">
+      <c r="C7" s="40" t="s">
         <v>13</v>
       </c>
     </row>
@@ -10544,7 +10524,7 @@
       <c r="B8" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="41" t="s">
+      <c r="C8" s="40" t="s">
         <v>15</v>
       </c>
     </row>
@@ -10555,7 +10535,7 @@
       <c r="B9" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="56" t="s">
+      <c r="C9" s="55" t="s">
         <v>17</v>
       </c>
     </row>
@@ -10569,7 +10549,7 @@
       <c r="C10" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="55" t="s">
+      <c r="D10" s="54" t="s">
         <v>20</v>
       </c>
     </row>
@@ -10604,7 +10584,7 @@
       <c r="C14" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="D14" s="41" t="s">
+      <c r="D14" s="40" t="s">
         <v>29</v>
       </c>
       <c r="E14" s="6" t="s">
@@ -10634,7 +10614,7 @@
       <c r="B17" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C17" s="41" t="s">
+      <c r="C17" s="40" t="s">
         <v>37</v>
       </c>
     </row>
@@ -10642,7 +10622,7 @@
       <c r="B18" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="C18" s="41" t="s">
+      <c r="C18" s="40" t="s">
         <v>39</v>
       </c>
     </row>
@@ -10670,10 +10650,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="21" t="s">
         <v>450</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="22" t="s">
         <v>451</v>
       </c>
     </row>
@@ -10781,7 +10761,7 @@
       </c>
     </row>
     <row r="16" spans="1:2">
-      <c r="A16" s="23" t="s">
+      <c r="A16" s="22" t="s">
         <v>477</v>
       </c>
       <c r="B16" t="s">
@@ -10854,7 +10834,7 @@
       </c>
     </row>
     <row r="28" spans="1:2" ht="75">
-      <c r="A28" s="61" t="s">
+      <c r="A28" s="64" t="s">
         <v>494</v>
       </c>
       <c r="B28" s="2" t="s">
@@ -10862,37 +10842,37 @@
       </c>
     </row>
     <row r="29" spans="1:2">
-      <c r="A29" s="61"/>
+      <c r="A29" s="64"/>
       <c r="B29" t="s">
         <v>496</v>
       </c>
     </row>
     <row r="30" spans="1:2">
-      <c r="A30" s="61"/>
+      <c r="A30" s="64"/>
       <c r="B30" t="s">
         <v>497</v>
       </c>
     </row>
     <row r="31" spans="1:2">
-      <c r="A31" s="61"/>
+      <c r="A31" s="64"/>
       <c r="B31" t="s">
         <v>498</v>
       </c>
     </row>
     <row r="32" spans="1:2">
-      <c r="A32" s="61"/>
+      <c r="A32" s="64"/>
       <c r="B32" t="s">
         <v>499</v>
       </c>
     </row>
     <row r="33" spans="1:2">
-      <c r="A33" s="61"/>
+      <c r="A33" s="64"/>
       <c r="B33" t="s">
         <v>500</v>
       </c>
     </row>
     <row r="34" spans="1:2">
-      <c r="A34" s="61"/>
+      <c r="A34" s="64"/>
       <c r="B34" t="s">
         <v>501</v>
       </c>
@@ -10907,240 +10887,227 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
-  <dimension ref="A1:C32"/>
+  <dimension ref="A1:C40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="26.25"/>
   <cols>
-    <col min="1" max="1" width="31.28515625" customWidth="1"/>
-    <col min="2" max="2" width="30.42578125" customWidth="1"/>
-    <col min="3" max="3" width="83" customWidth="1"/>
+    <col min="1" max="1" width="55.85546875" style="60" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="54.140625" style="61" customWidth="1"/>
+    <col min="3" max="3" width="101.7109375" style="93" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15" customHeight="1">
-      <c r="A1" s="88" t="s">
-        <v>749</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>517</v>
-      </c>
-      <c r="C1" s="18" t="s">
-        <v>518</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="15" customHeight="1">
-      <c r="A2" s="88"/>
-      <c r="B2" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="15" customHeight="1">
-      <c r="A3" s="88"/>
-      <c r="B3" t="s">
-        <v>503</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="15" customHeight="1">
-      <c r="A4" s="88"/>
-      <c r="B4" t="s">
-        <v>504</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="15" customHeight="1">
-      <c r="A5" s="88"/>
-      <c r="B5" t="s">
+    <row r="1" spans="1:3" ht="18.75">
+      <c r="A1" s="85" t="s">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15">
+      <c r="A2" s="85"/>
+      <c r="B2" s="86"/>
+      <c r="C2" s="94"/>
+    </row>
+    <row r="3" spans="1:3" ht="15">
+      <c r="A3" s="85"/>
+      <c r="B3" s="86"/>
+    </row>
+    <row r="4" spans="1:3" ht="15">
+      <c r="A4" s="85"/>
+      <c r="B4" s="86"/>
+    </row>
+    <row r="5" spans="1:3" ht="15">
+      <c r="A5" s="85"/>
+      <c r="B5" s="86"/>
+    </row>
+    <row r="6" spans="1:3" ht="15">
+      <c r="A6" s="85"/>
+      <c r="B6" s="86"/>
+    </row>
+    <row r="7" spans="1:3" ht="15">
+      <c r="A7" s="85"/>
+      <c r="B7" s="86"/>
+    </row>
+    <row r="8" spans="1:3" ht="15">
+      <c r="A8" s="85"/>
+      <c r="B8" s="86"/>
+    </row>
+    <row r="9" spans="1:3" ht="15">
+      <c r="A9" s="85"/>
+      <c r="B9" s="86"/>
+    </row>
+    <row r="10" spans="1:3" ht="15">
+      <c r="A10" s="85"/>
+      <c r="B10" s="86"/>
+    </row>
+    <row r="11" spans="1:3" ht="15">
+      <c r="A11" s="85"/>
+      <c r="B11" s="86"/>
+    </row>
+    <row r="12" spans="1:3" ht="15">
+      <c r="A12" s="85"/>
+      <c r="B12" s="86"/>
+    </row>
+    <row r="13" spans="1:3" ht="15">
+      <c r="A13" s="85"/>
+      <c r="B13" s="86"/>
+    </row>
+    <row r="14" spans="1:3" ht="15">
+      <c r="A14" s="85"/>
+      <c r="B14" s="86"/>
+    </row>
+    <row r="15" spans="1:3" ht="18.75" customHeight="1">
+      <c r="A15" s="85"/>
+      <c r="B15" s="86"/>
+    </row>
+    <row r="16" spans="1:3" ht="18.75" customHeight="1">
+      <c r="A16" s="85"/>
+      <c r="B16" s="86"/>
+    </row>
+    <row r="17" spans="1:3" ht="18.75" customHeight="1">
+      <c r="A17" s="85"/>
+      <c r="B17" s="86"/>
+    </row>
+    <row r="18" spans="1:3" ht="18.75" customHeight="1">
+      <c r="A18" s="85"/>
+      <c r="B18" s="86"/>
+    </row>
+    <row r="19" spans="1:3" ht="18.75" customHeight="1">
+      <c r="A19" s="85"/>
+      <c r="B19" s="86"/>
+    </row>
+    <row r="20" spans="1:3" ht="18.75" customHeight="1">
+      <c r="A20" s="85"/>
+      <c r="B20" s="86"/>
+    </row>
+    <row r="21" spans="1:3" ht="18.75" customHeight="1">
+      <c r="A21" s="85"/>
+      <c r="B21" s="86"/>
+    </row>
+    <row r="22" spans="1:3" ht="18.75">
+      <c r="A22" s="85"/>
+      <c r="B22" s="62"/>
+    </row>
+    <row r="23" spans="1:3" ht="18.75">
+      <c r="A23" s="85"/>
+      <c r="B23" s="62"/>
+    </row>
+    <row r="24" spans="1:3" ht="18.75">
+      <c r="A24" s="85"/>
+      <c r="B24" s="63"/>
+    </row>
+    <row r="26" spans="1:3" ht="18.75">
+      <c r="A26" s="85" t="s">
+        <v>727</v>
+      </c>
+      <c r="B26" s="61" t="s">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="18.75">
+      <c r="A27" s="85"/>
+      <c r="B27" s="61" t="s">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="18.75">
+      <c r="A28" s="85"/>
+      <c r="B28" s="61" t="s">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" s="59"/>
+    </row>
+    <row r="30" spans="1:3" ht="15">
+      <c r="A30" s="85" t="s">
+        <v>732</v>
+      </c>
+      <c r="B30" s="84" t="s">
         <v>505</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" ht="15" customHeight="1">
-      <c r="A6" s="88"/>
-      <c r="B6" t="s">
+      <c r="C30" s="93" t="s">
         <v>506</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15" customHeight="1">
-      <c r="A7" s="88"/>
-      <c r="B7" t="s">
+    <row r="31" spans="1:3" ht="15">
+      <c r="A31" s="85"/>
+      <c r="B31" s="84"/>
+      <c r="C31" s="93" t="s">
         <v>507</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="15" customHeight="1">
-      <c r="A8" s="88"/>
-      <c r="B8" t="s">
+    <row r="32" spans="1:3" ht="15">
+      <c r="A32" s="85"/>
+      <c r="B32" s="84"/>
+      <c r="C32" s="93" t="s">
         <v>508</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="15" customHeight="1">
-      <c r="A9" s="88"/>
-      <c r="B9" t="s">
+    <row r="33" spans="1:3" ht="15">
+      <c r="A33" s="85"/>
+      <c r="B33" s="84"/>
+      <c r="C33" s="93" t="s">
         <v>509</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="15" customHeight="1">
-      <c r="A10" s="88"/>
-      <c r="B10" t="s">
-        <v>510</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="15" customHeight="1">
-      <c r="A11" s="88"/>
-      <c r="B11" t="s">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="15" customHeight="1">
-      <c r="A12" s="88"/>
-      <c r="B12" s="91" t="s">
-        <v>750</v>
-      </c>
-      <c r="C12" t="s">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="15" customHeight="1">
-      <c r="A13" s="88"/>
-      <c r="B13" s="91"/>
-      <c r="C13" t="s">
-        <v>513</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="15" customHeight="1">
-      <c r="A14" s="88"/>
-      <c r="B14" s="91"/>
-      <c r="C14" t="s">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="15" customHeight="1">
-      <c r="A15" s="88"/>
-      <c r="B15" s="91"/>
-      <c r="C15" t="s">
-        <v>515</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="15" customHeight="1">
-      <c r="A16" s="88"/>
-      <c r="B16" s="91"/>
-      <c r="C16" t="s">
-        <v>516</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" s="88" t="s">
-        <v>742</v>
-      </c>
-      <c r="B18" s="89" t="s">
-        <v>746</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" s="88"/>
-      <c r="B19" s="89" t="s">
-        <v>744</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" s="88"/>
-      <c r="B20" s="89" t="s">
-        <v>745</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="15.75">
-      <c r="A21" s="90"/>
-      <c r="B21" s="89"/>
-    </row>
-    <row r="22" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A22" s="88" t="s">
-        <v>747</v>
-      </c>
-      <c r="B22" s="61" t="s">
-        <v>520</v>
-      </c>
-      <c r="C22" t="s">
-        <v>521</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A23" s="88"/>
-      <c r="B23" s="61"/>
-      <c r="C23" t="s">
-        <v>522</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A24" s="88"/>
-      <c r="B24" s="61"/>
-      <c r="C24" t="s">
-        <v>523</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A25" s="88"/>
-      <c r="B25" s="61"/>
-      <c r="C25" t="s">
-        <v>524</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="180">
-      <c r="A27" s="88" t="s">
-        <v>743</v>
-      </c>
-      <c r="B27" s="9" t="s">
-        <v>639</v>
-      </c>
-      <c r="C27" s="60" t="s">
-        <v>640</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="120">
-      <c r="A28" s="88"/>
-      <c r="B28" s="9" t="s">
-        <v>641</v>
-      </c>
-      <c r="C28" s="87" t="s">
-        <v>642</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="120">
-      <c r="A29" s="88"/>
-      <c r="B29" s="9" t="s">
-        <v>643</v>
-      </c>
-      <c r="C29" s="11" t="s">
-        <v>644</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="75">
-      <c r="A30" s="88"/>
-      <c r="B30" s="9" t="s">
-        <v>645</v>
-      </c>
-      <c r="C30" s="11" t="s">
-        <v>646</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="15.75">
-      <c r="A32" s="90" t="s">
-        <v>748</v>
+    <row r="35" spans="1:3" ht="210">
+      <c r="A35" s="85" t="s">
+        <v>728</v>
+      </c>
+      <c r="B35" s="61" t="s">
+        <v>624</v>
+      </c>
+      <c r="C35" s="95" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="135">
+      <c r="A36" s="85"/>
+      <c r="B36" s="61" t="s">
+        <v>626</v>
+      </c>
+      <c r="C36" s="95" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="120">
+      <c r="A37" s="85"/>
+      <c r="B37" s="61" t="s">
+        <v>628</v>
+      </c>
+      <c r="C37" s="96" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="90">
+      <c r="A38" s="85"/>
+      <c r="B38" s="61" t="s">
+        <v>630</v>
+      </c>
+      <c r="C38" s="96" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" s="59" t="s">
+        <v>733</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="B22:B25"/>
-    <mergeCell ref="A27:A30"/>
-    <mergeCell ref="A18:A20"/>
-    <mergeCell ref="A22:A25"/>
-    <mergeCell ref="B12:B16"/>
-    <mergeCell ref="A1:A16"/>
+  <mergeCells count="7">
+    <mergeCell ref="B30:B33"/>
+    <mergeCell ref="A35:A38"/>
+    <mergeCell ref="A26:A28"/>
+    <mergeCell ref="A30:A33"/>
+    <mergeCell ref="A1:A24"/>
+    <mergeCell ref="B2:B13"/>
+    <mergeCell ref="B14:B21"/>
   </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="C1" r:id="rId1" xr:uid="{F5CF4852-5086-49AF-9416-DCA12FECF90E}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -11159,287 +11126,287 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="150">
-      <c r="A1" s="17" t="s">
-        <v>525</v>
-      </c>
-      <c r="B1" s="57" t="s">
-        <v>526</v>
-      </c>
-      <c r="C1" s="18" t="s">
-        <v>527</v>
+      <c r="A1" s="16" t="s">
+        <v>510</v>
+      </c>
+      <c r="B1" s="56" t="s">
+        <v>511</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>512</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="200.25" customHeight="1">
       <c r="A2" s="6" t="s">
-        <v>528</v>
+        <v>513</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>529</v>
+        <v>514</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="120">
       <c r="A3" s="6" t="s">
-        <v>530</v>
+        <v>515</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>531</v>
+        <v>516</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="45">
       <c r="A4" s="6" t="s">
-        <v>532</v>
-      </c>
-      <c r="B4" s="57" t="s">
-        <v>533</v>
+        <v>517</v>
+      </c>
+      <c r="B4" s="56" t="s">
+        <v>518</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="30">
       <c r="A5" s="6" t="s">
-        <v>534</v>
+        <v>519</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>535</v>
+        <v>520</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="45">
       <c r="A6" s="6" t="s">
-        <v>536</v>
+        <v>521</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="45">
       <c r="A7" s="6" t="s">
-        <v>537</v>
+        <v>522</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>538</v>
+        <v>523</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="150">
       <c r="A8" s="6" t="s">
-        <v>539</v>
+        <v>524</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>540</v>
+        <v>525</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="60">
       <c r="A12" s="6" t="s">
-        <v>541</v>
+        <v>526</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>542</v>
+        <v>527</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="60">
       <c r="A13" s="6" t="s">
-        <v>543</v>
+        <v>528</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>544</v>
+        <v>529</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="120">
       <c r="A14" s="6" t="s">
-        <v>545</v>
+        <v>530</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>546</v>
+        <v>531</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="120">
       <c r="A15" s="6" t="s">
-        <v>547</v>
+        <v>532</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>548</v>
+        <v>533</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="6" t="s">
-        <v>549</v>
+        <v>534</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>550</v>
+        <v>535</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="225">
       <c r="A17" s="6" t="s">
-        <v>551</v>
+        <v>536</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>552</v>
+        <v>537</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="30">
       <c r="A18" s="6" t="s">
-        <v>553</v>
+        <v>538</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>554</v>
+        <v>539</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="345">
       <c r="A19" s="6" t="s">
-        <v>555</v>
+        <v>540</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>556</v>
+        <v>541</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="6" t="s">
-        <v>557</v>
+        <v>542</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="6" t="s">
-        <v>519</v>
+        <v>504</v>
       </c>
     </row>
     <row r="23" spans="1:2">
-      <c r="B23" s="19"/>
+      <c r="B23" s="18"/>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="6" t="s">
-        <v>558</v>
+        <v>543</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" s="6" t="s">
-        <v>559</v>
+        <v>544</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" s="6" t="s">
-        <v>560</v>
+        <v>545</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>561</v>
+        <v>546</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="45">
       <c r="A33" s="6" t="s">
-        <v>562</v>
+        <v>547</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>563</v>
+        <v>548</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="135">
       <c r="A34" s="6" t="s">
-        <v>564</v>
+        <v>549</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>565</v>
+        <v>550</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" s="6" t="s">
-        <v>566</v>
+        <v>551</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" s="6" t="s">
-        <v>567</v>
+        <v>552</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40" s="6" t="s">
-        <v>568</v>
+        <v>553</v>
       </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" s="6" t="s">
-        <v>569</v>
+        <v>554</v>
       </c>
     </row>
     <row r="44" spans="1:2">
       <c r="A44" s="6" t="s">
-        <v>570</v>
+        <v>555</v>
       </c>
     </row>
     <row r="46" spans="1:2">
       <c r="A46" s="6" t="s">
-        <v>571</v>
+        <v>556</v>
       </c>
     </row>
     <row r="48" spans="1:2">
       <c r="A48" s="6" t="s">
-        <v>572</v>
+        <v>557</v>
       </c>
     </row>
     <row r="50" spans="1:2">
       <c r="A50" s="6" t="s">
-        <v>573</v>
+        <v>558</v>
       </c>
     </row>
     <row r="52" spans="1:2">
       <c r="A52" s="6" t="s">
-        <v>574</v>
+        <v>559</v>
       </c>
     </row>
     <row r="54" spans="1:2">
-      <c r="A54" s="81" t="s">
-        <v>575</v>
+      <c r="A54" s="87" t="s">
+        <v>560</v>
       </c>
       <c r="B54" s="6" t="s">
-        <v>576</v>
+        <v>561</v>
       </c>
     </row>
     <row r="55" spans="1:2">
-      <c r="A55" s="81"/>
+      <c r="A55" s="87"/>
       <c r="B55" s="6" t="s">
-        <v>577</v>
+        <v>562</v>
       </c>
     </row>
     <row r="56" spans="1:2">
-      <c r="A56" s="81"/>
+      <c r="A56" s="87"/>
       <c r="B56" s="6" t="s">
-        <v>578</v>
+        <v>563</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="30">
-      <c r="A58" s="62" t="s">
-        <v>579</v>
+      <c r="A58" s="65" t="s">
+        <v>564</v>
       </c>
       <c r="B58" s="6" t="s">
-        <v>580</v>
+        <v>565</v>
       </c>
     </row>
     <row r="59" spans="1:2">
-      <c r="A59" s="62"/>
-      <c r="B59" s="21" t="s">
-        <v>581</v>
+      <c r="A59" s="65"/>
+      <c r="B59" s="20" t="s">
+        <v>566</v>
       </c>
     </row>
     <row r="60" spans="1:2">
-      <c r="A60" s="62"/>
-      <c r="B60" s="21" t="s">
-        <v>582</v>
+      <c r="A60" s="65"/>
+      <c r="B60" s="20" t="s">
+        <v>567</v>
       </c>
     </row>
     <row r="61" spans="1:2">
-      <c r="A61" s="62"/>
-      <c r="B61" s="21" t="s">
-        <v>583</v>
+      <c r="A61" s="65"/>
+      <c r="B61" s="20" t="s">
+        <v>568</v>
       </c>
     </row>
     <row r="62" spans="1:2">
-      <c r="A62" s="62"/>
-      <c r="B62" s="21" t="s">
-        <v>584</v>
+      <c r="A62" s="65"/>
+      <c r="B62" s="20" t="s">
+        <v>569</v>
       </c>
     </row>
     <row r="63" spans="1:2">
-      <c r="A63" s="62"/>
-      <c r="B63" s="21" t="s">
-        <v>585</v>
+      <c r="A63" s="65"/>
+      <c r="B63" s="20" t="s">
+        <v>570</v>
       </c>
     </row>
     <row r="64" spans="1:2">
-      <c r="A64" s="62"/>
-      <c r="B64" s="21" t="s">
-        <v>586</v>
+      <c r="A64" s="65"/>
+      <c r="B64" s="20" t="s">
+        <v>571</v>
       </c>
     </row>
   </sheetData>
@@ -11469,277 +11436,277 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="105">
-      <c r="A1" s="61" t="s">
-        <v>506</v>
+      <c r="A1" s="64" t="s">
+        <v>502</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="105">
+      <c r="A2" s="64"/>
+      <c r="B2" s="11" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="135">
+      <c r="A3" s="64"/>
+      <c r="B3" s="2" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="90">
+      <c r="A4" s="64" t="s">
+        <v>575</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="75">
+      <c r="A5" s="64"/>
+      <c r="B5" s="11" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="64"/>
+      <c r="B6" s="11" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="60">
+      <c r="A7" s="64" t="s">
+        <v>579</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="45">
+      <c r="A8" s="64"/>
+      <c r="B8" s="11" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="64"/>
+      <c r="B9" s="11" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="64"/>
+      <c r="B10" s="11" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="64"/>
+      <c r="B11" s="11" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="60">
+      <c r="A12" s="64" t="s">
+        <v>585</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="90">
+      <c r="A13" s="64"/>
+      <c r="B13" s="11" t="s">
         <v>587</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="105">
-      <c r="A2" s="61"/>
-      <c r="B2" s="12" t="s">
+    <row r="14" spans="1:2" ht="165">
+      <c r="A14" s="64"/>
+      <c r="B14" s="11" t="s">
         <v>588</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="135">
-      <c r="A3" s="61"/>
-      <c r="B3" s="2" t="s">
+    <row r="15" spans="1:2">
+      <c r="A15" s="64"/>
+      <c r="B15" s="11" t="s">
         <v>589</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="90">
-      <c r="A4" s="61" t="s">
+    <row r="16" spans="1:2">
+      <c r="A16" s="64"/>
+      <c r="B16" s="11" t="s">
         <v>590</v>
       </c>
-      <c r="B4" s="2" t="s">
+    </row>
+    <row r="17" spans="1:2" ht="120">
+      <c r="A17" s="64"/>
+      <c r="B17" s="11" t="s">
         <v>591</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="75">
-      <c r="A5" s="61"/>
-      <c r="B5" s="12" t="s">
+    <row r="18" spans="1:2" ht="60">
+      <c r="A18" s="64"/>
+      <c r="B18" s="11" t="s">
         <v>592</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
-      <c r="A6" s="61"/>
-      <c r="B6" s="12" t="s">
+    <row r="19" spans="1:2">
+      <c r="A19" s="64"/>
+      <c r="B19" s="11" t="s">
         <v>593</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="60">
-      <c r="A7" s="61" t="s">
+    <row r="20" spans="1:2">
+      <c r="A20" s="64"/>
+      <c r="B20" s="12" t="s">
         <v>594</v>
       </c>
-      <c r="B7" s="12" t="s">
+    </row>
+    <row r="21" spans="1:2" ht="195">
+      <c r="A21" s="89" t="s">
         <v>595</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" ht="45">
-      <c r="A8" s="61"/>
-      <c r="B8" s="12" t="s">
+      <c r="B21" s="11" t="s">
         <v>596</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
-      <c r="A9" s="61"/>
-      <c r="B9" s="12" t="s">
+    <row r="22" spans="1:2" ht="300">
+      <c r="A22" s="89"/>
+      <c r="B22" s="11" t="s">
         <v>597</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
-      <c r="A10" s="61"/>
-      <c r="B10" s="12" t="s">
+    <row r="23" spans="1:2" ht="195">
+      <c r="A23" s="89"/>
+      <c r="B23" s="11" t="s">
         <v>598</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
-      <c r="A11" s="61"/>
-      <c r="B11" s="12" t="s">
+    <row r="24" spans="1:2" ht="45">
+      <c r="A24" s="89"/>
+      <c r="B24" s="11" t="s">
         <v>599</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="60">
-      <c r="A12" s="61" t="s">
+    <row r="25" spans="1:2" ht="45">
+      <c r="A25" s="89"/>
+      <c r="B25" s="11" t="s">
         <v>600</v>
       </c>
-      <c r="B12" s="12" t="s">
+    </row>
+    <row r="26" spans="1:2" ht="75">
+      <c r="A26" s="89"/>
+      <c r="B26" s="11" t="s">
         <v>601</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="90">
-      <c r="A13" s="61"/>
-      <c r="B13" s="12" t="s">
+    <row r="27" spans="1:2">
+      <c r="A27" s="89"/>
+      <c r="B27" s="11" t="s">
         <v>602</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="165">
-      <c r="A14" s="61"/>
-      <c r="B14" s="12" t="s">
+    <row r="28" spans="1:2">
+      <c r="A28" s="89"/>
+      <c r="B28" s="12" t="s">
         <v>603</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
-      <c r="A15" s="61"/>
-      <c r="B15" s="12" t="s">
+    <row r="29" spans="1:2" ht="45">
+      <c r="A29" s="88" t="s">
         <v>604</v>
       </c>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16" s="61"/>
-      <c r="B16" s="12" t="s">
+      <c r="B29" s="11" t="s">
         <v>605</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="120">
-      <c r="A17" s="61"/>
-      <c r="B17" s="12" t="s">
+    <row r="30" spans="1:2">
+      <c r="A30" s="64"/>
+      <c r="B30" s="11" t="s">
         <v>606</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="60">
-      <c r="A18" s="61"/>
-      <c r="B18" s="12" t="s">
+    <row r="31" spans="1:2">
+      <c r="A31" s="64"/>
+      <c r="B31" s="11" t="s">
         <v>607</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
-      <c r="A19" s="61"/>
-      <c r="B19" s="12" t="s">
+    <row r="32" spans="1:2">
+      <c r="A32" s="64"/>
+      <c r="B32" s="11" t="s">
         <v>608</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
-      <c r="A20" s="61"/>
-      <c r="B20" s="13" t="s">
+    <row r="33" spans="1:2">
+      <c r="A33" s="64"/>
+      <c r="B33" s="11" t="s">
         <v>609</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="195">
-      <c r="A21" s="82" t="s">
+    <row r="34" spans="1:2" ht="75">
+      <c r="A34" s="89" t="s">
         <v>610</v>
       </c>
-      <c r="B21" s="12" t="s">
+      <c r="B34" s="2" t="s">
         <v>611</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="300">
-      <c r="A22" s="82"/>
-      <c r="B22" s="12" t="s">
+    <row r="35" spans="1:2" ht="60">
+      <c r="A35" s="64"/>
+      <c r="B35" s="2" t="s">
         <v>612</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="195">
-      <c r="A23" s="82"/>
-      <c r="B23" s="12" t="s">
+    <row r="36" spans="1:2" ht="75">
+      <c r="A36" s="64"/>
+      <c r="B36" s="2" t="s">
         <v>613</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="45">
-      <c r="A24" s="82"/>
-      <c r="B24" s="12" t="s">
+    <row r="37" spans="1:2" ht="75">
+      <c r="A37" s="64"/>
+      <c r="B37" s="2" t="s">
         <v>614</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="45">
-      <c r="A25" s="82"/>
-      <c r="B25" s="12" t="s">
+    <row r="38" spans="1:2" ht="45">
+      <c r="A38" s="64" t="s">
         <v>615</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" ht="75">
-      <c r="A26" s="82"/>
-      <c r="B26" s="12" t="s">
+      <c r="B38" s="2" t="s">
         <v>616</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
-      <c r="A27" s="82"/>
-      <c r="B27" s="12" t="s">
+    <row r="39" spans="1:2" ht="90">
+      <c r="A39" s="64"/>
+      <c r="B39" s="2" t="s">
         <v>617</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
-      <c r="A28" s="82"/>
-      <c r="B28" s="13" t="s">
+    <row r="40" spans="1:2" ht="30">
+      <c r="A40" s="64"/>
+      <c r="B40" s="2" t="s">
         <v>618</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="45">
-      <c r="A29" s="83" t="s">
+    <row r="41" spans="1:2" ht="30">
+      <c r="A41" s="64"/>
+      <c r="B41" s="2" t="s">
         <v>619</v>
       </c>
-      <c r="B29" s="12" t="s">
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42" s="64"/>
+      <c r="B42" s="2" t="s">
         <v>620</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
-      <c r="A30" s="61"/>
-      <c r="B30" s="12" t="s">
+    <row r="43" spans="1:2" ht="30">
+      <c r="A43" s="64"/>
+      <c r="B43" s="2" t="s">
         <v>621</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2">
-      <c r="A31" s="61"/>
-      <c r="B31" s="12" t="s">
-        <v>622</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2">
-      <c r="A32" s="61"/>
-      <c r="B32" s="12" t="s">
-        <v>623</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2">
-      <c r="A33" s="61"/>
-      <c r="B33" s="12" t="s">
-        <v>624</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" ht="75">
-      <c r="A34" s="82" t="s">
-        <v>625</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>626</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" ht="60">
-      <c r="A35" s="61"/>
-      <c r="B35" s="2" t="s">
-        <v>627</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" ht="75">
-      <c r="A36" s="61"/>
-      <c r="B36" s="2" t="s">
-        <v>628</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" ht="75">
-      <c r="A37" s="61"/>
-      <c r="B37" s="2" t="s">
-        <v>629</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" ht="45">
-      <c r="A38" s="61" t="s">
-        <v>630</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>631</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" ht="90">
-      <c r="A39" s="61"/>
-      <c r="B39" s="2" t="s">
-        <v>632</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" ht="30">
-      <c r="A40" s="61"/>
-      <c r="B40" s="2" t="s">
-        <v>633</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" ht="30">
-      <c r="A41" s="61"/>
-      <c r="B41" s="2" t="s">
-        <v>634</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2">
-      <c r="A42" s="61"/>
-      <c r="B42" s="2" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" ht="30">
-      <c r="A43" s="61"/>
-      <c r="B43" s="2" t="s">
-        <v>636</v>
       </c>
     </row>
     <row r="44" spans="1:2">
@@ -11748,10 +11715,10 @@
     </row>
     <row r="45" spans="1:2" ht="30">
       <c r="A45" s="4" t="s">
-        <v>637</v>
-      </c>
-      <c r="B45" s="16" t="s">
-        <v>638</v>
+        <v>622</v>
+      </c>
+      <c r="B45" s="15" t="s">
+        <v>623</v>
       </c>
     </row>
   </sheetData>
@@ -11790,18 +11757,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="135">
       <c r="A1" s="6" t="s">
-        <v>647</v>
-      </c>
-      <c r="B1" s="57" t="s">
-        <v>648</v>
+        <v>632</v>
+      </c>
+      <c r="B1" s="56" t="s">
+        <v>633</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="210">
       <c r="A2" s="5" t="s">
-        <v>649</v>
+        <v>634</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>650</v>
+        <v>635</v>
       </c>
     </row>
   </sheetData>
@@ -11853,22 +11820,22 @@
   <sheetData>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>651</v>
+        <v>636</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>652</v>
+        <v>637</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>653</v>
+        <v>638</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" t="s">
-        <v>654</v>
+        <v>639</v>
       </c>
     </row>
   </sheetData>
@@ -11893,146 +11860,146 @@
   <sheetData>
     <row r="1" spans="1:3" ht="26.25" customHeight="1">
       <c r="A1" s="7" t="s">
-        <v>655</v>
+        <v>640</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>656</v>
+        <v>641</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="4"/>
     </row>
     <row r="3" spans="1:3" ht="180">
-      <c r="A3" s="84" t="s">
+      <c r="A3" s="90" t="s">
+        <v>642</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>643</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="150">
+      <c r="A4" s="90"/>
+      <c r="B4" s="9" t="s">
+        <v>645</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="90"/>
+      <c r="B5" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="90"/>
+      <c r="B6" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="90"/>
+      <c r="B7" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="90">
+      <c r="A8" s="90"/>
+      <c r="B8" s="91" t="s">
+        <v>650</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="165">
+      <c r="A9" s="90"/>
+      <c r="B9" s="91"/>
+      <c r="C9" s="2" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="105">
+      <c r="A10" s="90"/>
+      <c r="B10" s="91"/>
+      <c r="C10" s="2" t="s">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="90"/>
+      <c r="B11" s="91"/>
+      <c r="C11" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="90">
+      <c r="A12" s="90"/>
+      <c r="B12" s="91"/>
+      <c r="C12" s="2" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="90"/>
+      <c r="B13" t="s">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="270">
+      <c r="A14" s="90"/>
+      <c r="B14" s="76" t="s">
         <v>657</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="C14" s="2" t="s">
         <v>658</v>
       </c>
-      <c r="C3" s="2" t="s">
+    </row>
+    <row r="15" spans="1:3" ht="210">
+      <c r="A15" s="90"/>
+      <c r="B15" s="76"/>
+      <c r="C15" s="11" t="s">
         <v>659</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="150">
-      <c r="A4" s="84"/>
-      <c r="B4" s="9" t="s">
+    <row r="16" spans="1:3" ht="120">
+      <c r="A16" s="90"/>
+      <c r="B16" s="76"/>
+      <c r="C16" s="11" t="s">
         <v>660</v>
       </c>
-      <c r="C4" s="2" t="s">
+    </row>
+    <row r="17" spans="1:6" ht="45">
+      <c r="A17" s="90"/>
+      <c r="B17" s="76"/>
+      <c r="C17" s="11" t="s">
         <v>661</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="84"/>
-      <c r="B5" t="s">
+    <row r="18" spans="1:6" ht="90">
+      <c r="A18" s="90"/>
+      <c r="B18" s="76"/>
+      <c r="C18" s="2" t="s">
         <v>662</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="84"/>
-      <c r="B6" t="s">
+    <row r="19" spans="1:6">
+      <c r="A19" s="90"/>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="90"/>
+      <c r="B20" s="12" t="s">
         <v>663</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="84"/>
-      <c r="B7" t="s">
+    <row r="21" spans="1:6">
+      <c r="A21" s="90"/>
+      <c r="B21" t="s">
         <v>664</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="90">
-      <c r="A8" s="84"/>
-      <c r="B8" s="85" t="s">
-        <v>665</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>666</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="165">
-      <c r="A9" s="84"/>
-      <c r="B9" s="85"/>
-      <c r="C9" s="2" t="s">
-        <v>667</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="105">
-      <c r="A10" s="84"/>
-      <c r="B10" s="85"/>
-      <c r="C10" s="2" t="s">
-        <v>668</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" s="84"/>
-      <c r="B11" s="85"/>
-      <c r="C11" t="s">
-        <v>669</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="90">
-      <c r="A12" s="84"/>
-      <c r="B12" s="85"/>
-      <c r="C12" s="2" t="s">
-        <v>670</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" s="84"/>
-      <c r="B13" t="s">
-        <v>671</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="270">
-      <c r="A14" s="84"/>
-      <c r="B14" s="73" t="s">
-        <v>672</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>673</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="210">
-      <c r="A15" s="84"/>
-      <c r="B15" s="73"/>
-      <c r="C15" s="12" t="s">
-        <v>674</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="120">
-      <c r="A16" s="84"/>
-      <c r="B16" s="73"/>
-      <c r="C16" s="12" t="s">
-        <v>675</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="45">
-      <c r="A17" s="84"/>
-      <c r="B17" s="73"/>
-      <c r="C17" s="12" t="s">
-        <v>676</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="90">
-      <c r="A18" s="84"/>
-      <c r="B18" s="73"/>
-      <c r="C18" s="2" t="s">
-        <v>677</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
-      <c r="A19" s="84"/>
-    </row>
-    <row r="20" spans="1:6">
-      <c r="A20" s="84"/>
-      <c r="B20" s="13" t="s">
-        <v>678</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
-      <c r="A21" s="84"/>
-      <c r="B21" t="s">
-        <v>679</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -12042,83 +12009,83 @@
       <c r="A23" s="4"/>
     </row>
     <row r="24" spans="1:6">
-      <c r="A24" s="84" t="s">
-        <v>680</v>
+      <c r="A24" s="90" t="s">
+        <v>665</v>
       </c>
       <c r="B24" t="s">
-        <v>681</v>
+        <v>666</v>
       </c>
     </row>
     <row r="25" spans="1:6">
-      <c r="A25" s="84"/>
+      <c r="A25" s="90"/>
       <c r="B25" t="s">
-        <v>682</v>
+        <v>667</v>
       </c>
     </row>
     <row r="26" spans="1:6">
-      <c r="A26" s="84"/>
+      <c r="A26" s="90"/>
       <c r="B26" t="s">
-        <v>683</v>
+        <v>668</v>
       </c>
     </row>
     <row r="27" spans="1:6">
-      <c r="A27" s="84"/>
+      <c r="A27" s="90"/>
       <c r="B27" t="s">
-        <v>684</v>
+        <v>669</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="90">
-      <c r="A28" s="84"/>
+      <c r="A28" s="90"/>
       <c r="B28" s="2" t="s">
-        <v>685</v>
+        <v>670</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="180">
-      <c r="A29" s="84"/>
+      <c r="A29" s="90"/>
       <c r="B29" s="2" t="s">
-        <v>686</v>
+        <v>671</v>
       </c>
     </row>
     <row r="30" spans="1:6">
-      <c r="A30" s="14"/>
+      <c r="A30" s="13"/>
     </row>
     <row r="31" spans="1:6" ht="180">
-      <c r="A31" s="84" t="s">
-        <v>687</v>
+      <c r="A31" s="90" t="s">
+        <v>672</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>688</v>
-      </c>
-      <c r="F31" s="15"/>
+        <v>673</v>
+      </c>
+      <c r="F31" s="14"/>
     </row>
     <row r="32" spans="1:6" ht="75">
-      <c r="A32" s="84"/>
+      <c r="A32" s="90"/>
       <c r="B32" s="2" t="s">
-        <v>689</v>
+        <v>674</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="30">
-      <c r="A33" s="84"/>
+      <c r="A33" s="90"/>
       <c r="B33" s="2" t="s">
-        <v>690</v>
+        <v>675</v>
       </c>
     </row>
     <row r="34" spans="1:3">
-      <c r="A34" s="84"/>
+      <c r="A34" s="90"/>
       <c r="B34" s="2" t="s">
-        <v>691</v>
+        <v>676</v>
       </c>
     </row>
     <row r="35" spans="1:3">
-      <c r="A35" s="84"/>
+      <c r="A35" s="90"/>
       <c r="B35" s="2" t="s">
-        <v>692</v>
+        <v>677</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="150">
-      <c r="A36" s="84"/>
+      <c r="A36" s="90"/>
       <c r="B36" s="2" t="s">
-        <v>693</v>
+        <v>678</v>
       </c>
       <c r="C36" s="2"/>
     </row>
@@ -12164,7 +12131,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="45">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="19" t="s">
         <v>40</v>
       </c>
       <c r="B1" s="6" t="s">
@@ -12172,7 +12139,7 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="45">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="19" t="s">
         <v>42</v>
       </c>
       <c r="B2" s="6" t="s">
@@ -12180,26 +12147,26 @@
       </c>
     </row>
     <row r="3" spans="1:2" ht="45">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="B3" s="57" t="s">
+      <c r="B3" s="56" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="360">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="B4" s="56" t="s">
+      <c r="B4" s="55" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="45">
-      <c r="A5" s="20" t="s">
+      <c r="A5" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="B5" s="57" t="s">
+      <c r="B5" s="56" t="s">
         <v>49</v>
       </c>
     </row>
@@ -12207,7 +12174,7 @@
       <c r="A6" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B6" s="57" t="s">
+      <c r="B6" s="56" t="s">
         <v>51</v>
       </c>
     </row>
@@ -12220,10 +12187,10 @@
       <c r="A8" s="4"/>
     </row>
     <row r="9" spans="1:2" ht="30">
-      <c r="A9" s="58" t="s">
+      <c r="A9" s="57" t="s">
         <v>53</v>
       </c>
-      <c r="B9" s="57" t="s">
+      <c r="B9" s="56" t="s">
         <v>54</v>
       </c>
     </row>
@@ -12234,60 +12201,60 @@
       <c r="A11" s="4"/>
     </row>
     <row r="12" spans="1:2" ht="195">
-      <c r="A12" s="20" t="s">
+      <c r="A12" s="19" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:2">
-      <c r="A13" s="42" t="s">
+      <c r="A13" s="41" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="14" spans="1:2">
-      <c r="A14" s="43" t="s">
+      <c r="A14" s="42" t="s">
         <v>57</v>
       </c>
-      <c r="B14" s="44" t="s">
+      <c r="B14" s="43" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:2">
-      <c r="A15" s="42" t="s">
+      <c r="A15" s="41" t="s">
         <v>59</v>
       </c>
-      <c r="B15" s="45" t="s">
+      <c r="B15" s="44" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="51">
-      <c r="A16" s="43" t="s">
+      <c r="A16" s="42" t="s">
         <v>61</v>
       </c>
-      <c r="B16" s="46" t="s">
+      <c r="B16" s="45" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="17" spans="1:2">
-      <c r="A17" s="42" t="s">
+      <c r="A17" s="41" t="s">
         <v>63</v>
       </c>
-      <c r="B17" s="25" t="s">
+      <c r="B17" s="24" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="18" spans="1:2">
-      <c r="A18" s="43" t="s">
+      <c r="A18" s="42" t="s">
         <v>65</v>
       </c>
-      <c r="B18" s="27" t="s">
+      <c r="B18" s="26" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="19" spans="1:2">
-      <c r="A19" s="42" t="s">
+      <c r="A19" s="41" t="s">
         <v>67</v>
       </c>
-      <c r="B19" s="25"/>
+      <c r="B19" s="24"/>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="4"/>
@@ -12410,7 +12377,7 @@
       </c>
     </row>
     <row r="40" spans="1:2" ht="45">
-      <c r="A40" s="61" t="s">
+      <c r="A40" s="64" t="s">
         <v>92</v>
       </c>
       <c r="B40" s="6" t="s">
@@ -12418,25 +12385,25 @@
       </c>
     </row>
     <row r="41" spans="1:2">
-      <c r="A41" s="61"/>
+      <c r="A41" s="64"/>
       <c r="B41" s="5" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="42" spans="1:2">
-      <c r="A42" s="61"/>
+      <c r="A42" s="64"/>
       <c r="B42" s="5" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="43" spans="1:2">
-      <c r="A43" s="61"/>
+      <c r="A43" s="64"/>
       <c r="B43" s="5" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="60">
-      <c r="A44" s="61" t="s">
+      <c r="A44" s="64" t="s">
         <v>97</v>
       </c>
       <c r="B44" s="6" t="s">
@@ -12444,13 +12411,13 @@
       </c>
     </row>
     <row r="45" spans="1:2" ht="60">
-      <c r="A45" s="61"/>
-      <c r="B45" s="21" t="s">
+      <c r="A45" s="64"/>
+      <c r="B45" s="20" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="75">
-      <c r="A46" s="61" t="s">
+      <c r="A46" s="64" t="s">
         <v>100</v>
       </c>
       <c r="B46" s="6" t="s">
@@ -12458,7 +12425,7 @@
       </c>
     </row>
     <row r="47" spans="1:2" ht="60">
-      <c r="A47" s="61"/>
+      <c r="A47" s="64"/>
       <c r="B47" s="6" t="s">
         <v>102</v>
       </c>
@@ -12488,7 +12455,7 @@
       </c>
     </row>
     <row r="51" spans="1:2" ht="90">
-      <c r="A51" s="62" t="s">
+      <c r="A51" s="65" t="s">
         <v>109</v>
       </c>
       <c r="B51" s="6" t="s">
@@ -12496,19 +12463,19 @@
       </c>
     </row>
     <row r="52" spans="1:2" ht="135">
-      <c r="A52" s="62"/>
+      <c r="A52" s="65"/>
       <c r="B52" s="6" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="105">
-      <c r="A53" s="62"/>
+      <c r="A53" s="65"/>
       <c r="B53" s="6" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="60">
-      <c r="A54" s="63" t="s">
+      <c r="A54" s="66" t="s">
         <v>113</v>
       </c>
       <c r="B54" s="6" t="s">
@@ -12516,38 +12483,38 @@
       </c>
     </row>
     <row r="55" spans="1:2" ht="120">
-      <c r="A55" s="63"/>
+      <c r="A55" s="66"/>
       <c r="B55" s="6" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="180">
-      <c r="A56" s="63"/>
-      <c r="B56" s="21" t="s">
+      <c r="A56" s="66"/>
+      <c r="B56" s="20" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="210">
-      <c r="A57" s="63"/>
-      <c r="B57" s="21" t="s">
+      <c r="A57" s="66"/>
+      <c r="B57" s="20" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="240">
-      <c r="A58" s="63"/>
+      <c r="A58" s="66"/>
       <c r="B58" s="6" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="90">
-      <c r="A59" s="63"/>
-      <c r="B59" s="47" t="s">
+      <c r="A59" s="66"/>
+      <c r="B59" s="46" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="409.5">
-      <c r="A60" s="63"/>
-      <c r="B60" s="48" t="s">
+      <c r="A60" s="66"/>
+      <c r="B60" s="47" t="s">
         <v>120</v>
       </c>
     </row>
@@ -12576,7 +12543,7 @@
       </c>
     </row>
     <row r="64" spans="1:2" ht="135">
-      <c r="A64" s="49" t="s">
+      <c r="A64" s="48" t="s">
         <v>127</v>
       </c>
       <c r="B64" s="6" t="s">
@@ -12584,7 +12551,7 @@
       </c>
     </row>
     <row r="65" spans="1:2" ht="165">
-      <c r="A65" s="64" t="s">
+      <c r="A65" s="68" t="s">
         <v>129</v>
       </c>
       <c r="B65" s="6" t="s">
@@ -12592,53 +12559,53 @@
       </c>
     </row>
     <row r="66" spans="1:2">
-      <c r="A66" s="64"/>
-      <c r="B66" s="50" t="s">
+      <c r="A66" s="68"/>
+      <c r="B66" s="49" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="67" spans="1:2">
-      <c r="A67" s="65" t="s">
+      <c r="A67" s="69" t="s">
         <v>132</v>
       </c>
-      <c r="B67" s="51" t="s">
+      <c r="B67" s="50" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="68" spans="1:2" ht="60">
-      <c r="A68" s="66"/>
-      <c r="B68" s="32" t="s">
+      <c r="A68" s="70"/>
+      <c r="B68" s="31" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="69" spans="1:2" ht="30">
-      <c r="A69" s="66"/>
-      <c r="B69" s="48" t="s">
+      <c r="A69" s="70"/>
+      <c r="B69" s="47" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="70" spans="1:2">
-      <c r="A70" s="66"/>
-      <c r="B70" s="51" t="s">
+      <c r="A70" s="70"/>
+      <c r="B70" s="50" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="71" spans="1:2" ht="60">
-      <c r="A71" s="61" t="s">
+      <c r="A71" s="64" t="s">
         <v>137</v>
       </c>
-      <c r="B71" s="21" t="s">
+      <c r="B71" s="20" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="72" spans="1:2">
-      <c r="A72" s="61"/>
-      <c r="B72" s="50" t="s">
+      <c r="A72" s="64"/>
+      <c r="B72" s="49" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="60">
-      <c r="A73" s="61"/>
+      <c r="A73" s="64"/>
       <c r="B73" s="6" t="s">
         <v>140</v>
       </c>
@@ -12652,7 +12619,7 @@
       </c>
     </row>
     <row r="75" spans="1:2" ht="60">
-      <c r="A75" s="61" t="s">
+      <c r="A75" s="64" t="s">
         <v>143</v>
       </c>
       <c r="B75" s="6" t="s">
@@ -12660,32 +12627,32 @@
       </c>
     </row>
     <row r="76" spans="1:2" ht="75">
-      <c r="A76" s="61"/>
+      <c r="A76" s="64"/>
       <c r="B76" s="6" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="77" spans="1:2" ht="75">
-      <c r="A77" s="61"/>
+      <c r="A77" s="64"/>
       <c r="B77" s="6" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="90">
-      <c r="A78" s="61"/>
+      <c r="A78" s="64"/>
       <c r="B78" s="6" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="79" spans="1:2" ht="75">
-      <c r="A79" s="61"/>
-      <c r="B79" s="21" t="s">
+      <c r="A79" s="64"/>
+      <c r="B79" s="20" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="80" spans="1:2">
-      <c r="A80" s="61"/>
-      <c r="B80" s="50" t="s">
+      <c r="A80" s="64"/>
+      <c r="B80" s="49" t="s">
         <v>149</v>
       </c>
     </row>
@@ -12700,93 +12667,93 @@
       </c>
     </row>
     <row r="83" spans="1:3">
-      <c r="A83" s="66" t="s">
+      <c r="A83" s="70" t="s">
         <v>152</v>
       </c>
       <c r="B83" s="67" t="s">
         <v>153</v>
       </c>
-      <c r="C83" s="53" t="s">
+      <c r="C83" s="52" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="84" spans="1:3">
-      <c r="A84" s="66"/>
+      <c r="A84" s="70"/>
       <c r="B84" s="67"/>
-      <c r="C84" s="53" t="s">
+      <c r="C84" s="52" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="85" spans="1:3">
-      <c r="A85" s="66"/>
+      <c r="A85" s="70"/>
       <c r="B85" s="67" t="s">
         <v>156</v>
       </c>
-      <c r="C85" s="53" t="s">
+      <c r="C85" s="52" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="86" spans="1:3">
-      <c r="A86" s="66"/>
+      <c r="A86" s="70"/>
       <c r="B86" s="67"/>
-      <c r="C86" s="53" t="s">
+      <c r="C86" s="52" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="87" spans="1:3">
-      <c r="A87" s="66"/>
-      <c r="B87" s="52" t="s">
+      <c r="A87" s="70"/>
+      <c r="B87" s="51" t="s">
         <v>158</v>
       </c>
-      <c r="C87" s="53" t="s">
+      <c r="C87" s="52" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="88" spans="1:3">
-      <c r="A88" s="66"/>
+      <c r="A88" s="70"/>
       <c r="B88" s="67" t="s">
         <v>160</v>
       </c>
-      <c r="C88" s="53" t="s">
+      <c r="C88" s="52" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="89" spans="1:3">
-      <c r="A89" s="66"/>
+      <c r="A89" s="70"/>
       <c r="B89" s="67"/>
-      <c r="C89" s="53" t="s">
+      <c r="C89" s="52" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="90" spans="1:3">
-      <c r="A90" s="66"/>
-      <c r="B90" s="52" t="s">
+      <c r="A90" s="70"/>
+      <c r="B90" s="51" t="s">
         <v>162</v>
       </c>
-      <c r="C90" s="53"/>
+      <c r="C90" s="52"/>
     </row>
     <row r="91" spans="1:3">
-      <c r="A91" s="66"/>
+      <c r="A91" s="70"/>
       <c r="B91" s="67" t="s">
         <v>163</v>
       </c>
-      <c r="C91" s="53" t="s">
+      <c r="C91" s="52" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="92" spans="1:3">
-      <c r="A92" s="66"/>
+      <c r="A92" s="70"/>
       <c r="B92" s="67"/>
-      <c r="C92" s="53" t="s">
+      <c r="C92" s="52" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="93" spans="1:3">
-      <c r="A93" s="66"/>
-      <c r="B93" s="52" t="s">
+      <c r="A93" s="70"/>
+      <c r="B93" s="51" t="s">
         <v>166</v>
       </c>
-      <c r="C93" s="53" t="s">
+      <c r="C93" s="52" t="s">
         <v>167</v>
       </c>
     </row>
@@ -12848,26 +12815,26 @@
   <sheetData>
     <row r="1" spans="1:2" ht="195">
       <c r="A1" s="5" t="s">
-        <v>694</v>
+        <v>679</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>695</v>
+        <v>680</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="90">
       <c r="A2" s="6" t="s">
-        <v>696</v>
+        <v>681</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>697</v>
+        <v>682</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="180">
       <c r="A3" s="6" t="s">
-        <v>698</v>
+        <v>683</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>699</v>
+        <v>684</v>
       </c>
     </row>
   </sheetData>
@@ -12905,96 +12872,96 @@
   <sheetData>
     <row r="2" spans="1:2" ht="75">
       <c r="A2" t="s">
-        <v>700</v>
+        <v>685</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>701</v>
+        <v>686</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="165">
       <c r="A3" t="s">
-        <v>702</v>
+        <v>687</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>703</v>
+        <v>688</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="150">
       <c r="A4" t="s">
-        <v>704</v>
+        <v>689</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>705</v>
+        <v>690</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="75">
       <c r="A5" t="s">
-        <v>515</v>
+        <v>503</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>706</v>
+        <v>691</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="60">
       <c r="A6" t="s">
-        <v>707</v>
+        <v>692</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>708</v>
+        <v>693</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="60">
       <c r="A7" t="s">
-        <v>709</v>
+        <v>694</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>710</v>
+        <v>695</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="75">
       <c r="A8" t="s">
-        <v>711</v>
+        <v>696</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>712</v>
+        <v>697</v>
       </c>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" s="61" t="s">
-        <v>713</v>
+      <c r="A9" s="64" t="s">
+        <v>698</v>
       </c>
       <c r="B9" t="s">
-        <v>714</v>
+        <v>699</v>
       </c>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" s="61"/>
+      <c r="A10" s="64"/>
       <c r="B10" t="s">
-        <v>715</v>
+        <v>700</v>
       </c>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" s="61"/>
+      <c r="A11" s="64"/>
       <c r="B11" t="s">
-        <v>716</v>
+        <v>701</v>
       </c>
     </row>
     <row r="12" spans="1:2">
-      <c r="A12" s="61"/>
+      <c r="A12" s="64"/>
       <c r="B12" t="s">
-        <v>717</v>
+        <v>702</v>
       </c>
     </row>
     <row r="13" spans="1:2">
-      <c r="A13" s="61"/>
+      <c r="A13" s="64"/>
       <c r="B13" t="s">
-        <v>718</v>
+        <v>703</v>
       </c>
     </row>
     <row r="14" spans="1:2">
-      <c r="A14" s="61"/>
+      <c r="A14" s="64"/>
       <c r="B14" t="s">
-        <v>719</v>
+        <v>704</v>
       </c>
     </row>
   </sheetData>
@@ -13022,110 +12989,110 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>720</v>
+        <v>705</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>721</v>
+        <v>706</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>722</v>
+        <v>707</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>723</v>
+        <v>708</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="75">
       <c r="A4" t="s">
-        <v>724</v>
+        <v>709</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>725</v>
+        <v>710</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="60">
       <c r="A6" t="s">
-        <v>726</v>
+        <v>711</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>727</v>
+        <v>712</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>728</v>
+        <v>713</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="45">
       <c r="A10" t="s">
-        <v>729</v>
+        <v>714</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>730</v>
+        <v>715</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>731</v>
+        <v>716</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>732</v>
+        <v>717</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
-        <v>733</v>
+        <v>718</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>734</v>
+        <v>719</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>735</v>
+        <v>720</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="3" t="s">
-        <v>736</v>
+        <v>721</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="105">
-      <c r="A27" s="86" t="s">
-        <v>737</v>
+      <c r="A27" s="92" t="s">
+        <v>722</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>738</v>
+        <v>723</v>
       </c>
     </row>
     <row r="28" spans="1:2">
-      <c r="A28" s="86"/>
+      <c r="A28" s="92"/>
       <c r="B28" t="s">
-        <v>739</v>
+        <v>724</v>
       </c>
     </row>
     <row r="29" spans="1:2">
-      <c r="A29" s="86"/>
+      <c r="A29" s="92"/>
       <c r="B29" t="s">
-        <v>740</v>
+        <v>725</v>
       </c>
     </row>
     <row r="30" spans="1:2">
-      <c r="A30" s="86"/>
+      <c r="A30" s="92"/>
       <c r="B30" t="s">
-        <v>741</v>
+        <v>726</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="B31" t="s">
-        <v>733</v>
+        <v>718</v>
       </c>
     </row>
   </sheetData>
@@ -13155,7 +13122,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="303" customHeight="1">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="19" t="s">
         <v>169</v>
       </c>
       <c r="B1" s="6" t="s">
@@ -13163,7 +13130,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="180">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="19" t="s">
         <v>171</v>
       </c>
       <c r="B2" s="6" t="s">
@@ -13171,7 +13138,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="90">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="19" t="s">
         <v>173</v>
       </c>
       <c r="B3" s="6" t="s">
@@ -13179,10 +13146,10 @@
       </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="68" t="s">
+      <c r="A4" s="71" t="s">
         <v>175</v>
       </c>
-      <c r="B4" s="25" t="s">
+      <c r="B4" s="24" t="s">
         <v>176</v>
       </c>
       <c r="E4" s="1" t="s">
@@ -13190,44 +13157,44 @@
       </c>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="69"/>
-      <c r="B5" s="27" t="s">
+      <c r="A5" s="72"/>
+      <c r="B5" s="26" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="69"/>
-      <c r="B6" s="25" t="s">
+      <c r="A6" s="72"/>
+      <c r="B6" s="24" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="69"/>
-      <c r="B7" s="27" t="s">
+      <c r="A7" s="72"/>
+      <c r="B7" s="26" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="69"/>
-      <c r="B8" s="25" t="s">
+      <c r="A8" s="72"/>
+      <c r="B8" s="24" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="69"/>
-      <c r="B9" s="27" t="s">
+      <c r="A9" s="72"/>
+      <c r="B9" s="26" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="69"/>
-      <c r="B10" s="25" t="s">
+      <c r="A10" s="72"/>
+      <c r="B10" s="24" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="70"/>
-      <c r="B11" s="27" t="s">
+      <c r="A11" s="73"/>
+      <c r="B11" s="26" t="s">
         <v>184</v>
       </c>
     </row>
@@ -13235,7 +13202,7 @@
       <c r="A12" s="4"/>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="20" t="s">
+      <c r="A13" s="19" t="s">
         <v>185</v>
       </c>
     </row>
@@ -13290,7 +13257,7 @@
       </c>
     </row>
     <row r="23" spans="1:3" ht="240">
-      <c r="A23" s="39" t="s">
+      <c r="A23" s="38" t="s">
         <v>194</v>
       </c>
       <c r="B23" s="2" t="s">
@@ -13333,7 +13300,7 @@
       <c r="A28" s="4" t="s">
         <v>204</v>
       </c>
-      <c r="B28" s="12" t="s">
+      <c r="B28" s="11" t="s">
         <v>205</v>
       </c>
     </row>
@@ -13354,29 +13321,29 @@
       </c>
     </row>
     <row r="31" spans="1:3">
-      <c r="A31" s="61" t="s">
+      <c r="A31" s="64" t="s">
         <v>210</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="C31" s="71" t="s">
+      <c r="C31" s="74" t="s">
         <v>212</v>
       </c>
     </row>
     <row r="32" spans="1:3">
-      <c r="A32" s="61"/>
+      <c r="A32" s="64"/>
       <c r="B32" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="C32" s="72"/>
+      <c r="C32" s="75"/>
     </row>
     <row r="33" spans="1:3" ht="135">
-      <c r="A33" s="61"/>
-      <c r="B33" s="40" t="s">
+      <c r="A33" s="64"/>
+      <c r="B33" s="39" t="s">
         <v>214</v>
       </c>
-      <c r="C33" s="72"/>
+      <c r="C33" s="75"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -13410,12 +13377,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="26.25">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="27" t="s">
         <v>215</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="192.75" customHeight="1">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="19" t="s">
         <v>216</v>
       </c>
       <c r="B2" s="6" t="s">
@@ -13423,15 +13390,15 @@
       </c>
     </row>
     <row r="3" spans="1:3" ht="105">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="19" t="s">
         <v>218</v>
       </c>
-      <c r="B3" s="57" t="s">
+      <c r="B3" s="56" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="45">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="19" t="s">
         <v>220</v>
       </c>
       <c r="B4" s="6" t="s">
@@ -13450,10 +13417,10 @@
       <c r="A6" s="4" t="s">
         <v>224</v>
       </c>
-      <c r="B6" s="24" t="s">
+      <c r="B6" s="23" t="s">
         <v>225</v>
       </c>
-      <c r="C6" s="18" t="s">
+      <c r="C6" s="17" t="s">
         <v>226</v>
       </c>
     </row>
@@ -13539,10 +13506,10 @@
       <c r="A23" s="4"/>
     </row>
     <row r="24" spans="1:2" ht="60">
-      <c r="A24" s="34" t="s">
+      <c r="A24" s="33" t="s">
         <v>238</v>
       </c>
-      <c r="B24" s="35" t="s">
+      <c r="B24" s="34" t="s">
         <v>239</v>
       </c>
     </row>
@@ -13573,7 +13540,7 @@
       <c r="A31" s="4"/>
     </row>
     <row r="32" spans="1:2" ht="26.25">
-      <c r="A32" s="28" t="s">
+      <c r="A32" s="27" t="s">
         <v>186</v>
       </c>
     </row>
@@ -13614,7 +13581,7 @@
       <c r="B37" s="2"/>
     </row>
     <row r="38" spans="1:2" ht="75">
-      <c r="A38" s="61" t="s">
+      <c r="A38" s="64" t="s">
         <v>250</v>
       </c>
       <c r="B38" s="2" t="s">
@@ -13622,25 +13589,25 @@
       </c>
     </row>
     <row r="39" spans="1:2" ht="90">
-      <c r="A39" s="61"/>
+      <c r="A39" s="64"/>
       <c r="B39" s="2" t="s">
         <v>252</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="45">
-      <c r="A40" s="61"/>
+      <c r="A40" s="64"/>
       <c r="B40" s="2" t="s">
         <v>253</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="135">
-      <c r="A41" s="61"/>
+      <c r="A41" s="64"/>
       <c r="B41" s="2" t="s">
         <v>254</v>
       </c>
     </row>
     <row r="42" spans="1:2">
-      <c r="A42" s="61"/>
+      <c r="A42" s="64"/>
     </row>
     <row r="43" spans="1:2">
       <c r="A43" s="4"/>
@@ -13679,7 +13646,7 @@
       <c r="A49" s="4"/>
     </row>
     <row r="50" spans="1:3">
-      <c r="A50" s="61" t="s">
+      <c r="A50" s="64" t="s">
         <v>260</v>
       </c>
       <c r="B50" t="s">
@@ -13687,13 +13654,13 @@
       </c>
     </row>
     <row r="51" spans="1:3" ht="30">
-      <c r="A51" s="61"/>
+      <c r="A51" s="64"/>
       <c r="B51" s="2" t="s">
         <v>262</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="30">
-      <c r="A52" s="61"/>
+      <c r="A52" s="64"/>
       <c r="B52" s="2" t="s">
         <v>263</v>
       </c>
@@ -13713,33 +13680,33 @@
       <c r="A55" s="4"/>
     </row>
     <row r="56" spans="1:3" ht="135">
-      <c r="A56" s="66" t="s">
+      <c r="A56" s="70" t="s">
         <v>266</v>
       </c>
-      <c r="B56" s="73" t="s">
+      <c r="B56" s="76" t="s">
         <v>267</v>
       </c>
-      <c r="C56" s="12" t="s">
+      <c r="C56" s="11" t="s">
         <v>268</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="75">
-      <c r="A57" s="66"/>
-      <c r="B57" s="73"/>
-      <c r="C57" s="12" t="s">
+      <c r="A57" s="70"/>
+      <c r="B57" s="76"/>
+      <c r="C57" s="11" t="s">
         <v>269</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="30">
-      <c r="A58" s="66"/>
-      <c r="B58" s="73"/>
-      <c r="C58" s="12" t="s">
+      <c r="A58" s="70"/>
+      <c r="B58" s="76"/>
+      <c r="C58" s="11" t="s">
         <v>270</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="180">
-      <c r="A59" s="66"/>
-      <c r="B59" s="73"/>
+      <c r="A59" s="70"/>
+      <c r="B59" s="76"/>
       <c r="C59" s="2" t="s">
         <v>271</v>
       </c>
@@ -13757,7 +13724,7 @@
       <c r="B61" s="2"/>
     </row>
     <row r="62" spans="1:3" ht="60">
-      <c r="A62" s="61" t="s">
+      <c r="A62" s="64" t="s">
         <v>274</v>
       </c>
       <c r="B62" s="2" t="s">
@@ -13765,25 +13732,25 @@
       </c>
     </row>
     <row r="63" spans="1:3" ht="150">
-      <c r="A63" s="61"/>
+      <c r="A63" s="64"/>
       <c r="B63" s="2" t="s">
         <v>276</v>
       </c>
     </row>
     <row r="64" spans="1:3" ht="75">
-      <c r="A64" s="61"/>
+      <c r="A64" s="64"/>
       <c r="B64" s="2" t="s">
         <v>277</v>
       </c>
     </row>
     <row r="65" spans="1:3" ht="90">
-      <c r="A65" s="61"/>
+      <c r="A65" s="64"/>
       <c r="B65" s="2" t="s">
         <v>278</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="75">
-      <c r="A66" s="61"/>
+      <c r="A66" s="64"/>
       <c r="B66" s="2" t="s">
         <v>279</v>
       </c>
@@ -13793,7 +13760,7 @@
       <c r="B67" s="2"/>
     </row>
     <row r="68" spans="1:3" ht="90">
-      <c r="A68" s="61" t="s">
+      <c r="A68" s="64" t="s">
         <v>280</v>
       </c>
       <c r="B68" s="2" t="s">
@@ -13801,13 +13768,13 @@
       </c>
     </row>
     <row r="69" spans="1:3" ht="75">
-      <c r="A69" s="61"/>
+      <c r="A69" s="64"/>
       <c r="B69" s="2" t="s">
         <v>282</v>
       </c>
     </row>
     <row r="70" spans="1:3">
-      <c r="A70" s="61"/>
+      <c r="A70" s="64"/>
       <c r="B70" s="2" t="s">
         <v>283</v>
       </c>
@@ -13816,7 +13783,7 @@
       <c r="A71" s="4"/>
     </row>
     <row r="72" spans="1:3" ht="30">
-      <c r="A72" s="34" t="s">
+      <c r="A72" s="33" t="s">
         <v>284</v>
       </c>
       <c r="B72" s="2" t="s">
@@ -13827,7 +13794,7 @@
       <c r="A73" s="4"/>
     </row>
     <row r="74" spans="1:3" ht="45">
-      <c r="A74" s="61" t="s">
+      <c r="A74" s="64" t="s">
         <v>286</v>
       </c>
       <c r="B74" s="2" t="s">
@@ -13835,37 +13802,37 @@
       </c>
     </row>
     <row r="75" spans="1:3" ht="45">
-      <c r="A75" s="61"/>
+      <c r="A75" s="64"/>
       <c r="B75" s="2" t="s">
         <v>288</v>
       </c>
     </row>
     <row r="76" spans="1:3" ht="60">
-      <c r="A76" s="61"/>
-      <c r="B76" s="12" t="s">
+      <c r="A76" s="64"/>
+      <c r="B76" s="11" t="s">
         <v>289</v>
       </c>
     </row>
     <row r="77" spans="1:3" ht="45">
-      <c r="A77" s="61"/>
-      <c r="B77" s="12" t="s">
+      <c r="A77" s="64"/>
+      <c r="B77" s="11" t="s">
         <v>290</v>
       </c>
     </row>
     <row r="78" spans="1:3" ht="90">
-      <c r="A78" s="61"/>
-      <c r="B78" s="12" t="s">
+      <c r="A78" s="64"/>
+      <c r="B78" s="11" t="s">
         <v>291</v>
       </c>
     </row>
     <row r="79" spans="1:3" ht="285">
-      <c r="A79" s="14" t="s">
+      <c r="A79" s="13" t="s">
         <v>292</v>
       </c>
       <c r="B79" s="2" t="s">
         <v>293</v>
       </c>
-      <c r="C79" s="36" t="s">
+      <c r="C79" s="35" t="s">
         <v>294</v>
       </c>
     </row>
@@ -13898,7 +13865,7 @@
       <c r="A89" s="4"/>
     </row>
     <row r="90" spans="1:2" ht="26.25">
-      <c r="A90" s="28" t="s">
+      <c r="A90" s="27" t="s">
         <v>300</v>
       </c>
     </row>
@@ -13906,7 +13873,7 @@
       <c r="A91" s="4"/>
     </row>
     <row r="92" spans="1:2" ht="135">
-      <c r="A92" s="61" t="s">
+      <c r="A92" s="64" t="s">
         <v>236</v>
       </c>
       <c r="B92" s="2" t="s">
@@ -13914,63 +13881,63 @@
       </c>
     </row>
     <row r="93" spans="1:2" ht="165">
-      <c r="A93" s="61"/>
+      <c r="A93" s="64"/>
       <c r="B93" s="2" t="s">
         <v>302</v>
       </c>
     </row>
     <row r="94" spans="1:2" ht="60">
-      <c r="A94" s="61" t="s">
+      <c r="A94" s="64" t="s">
         <v>303</v>
       </c>
-      <c r="B94" s="37" t="s">
+      <c r="B94" s="36" t="s">
         <v>304</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="225">
-      <c r="A95" s="61"/>
-      <c r="B95" s="38" t="s">
+      <c r="A95" s="64"/>
+      <c r="B95" s="37" t="s">
         <v>305</v>
       </c>
     </row>
     <row r="96" spans="1:2" ht="390">
-      <c r="A96" s="61"/>
-      <c r="B96" s="38" t="s">
+      <c r="A96" s="64"/>
+      <c r="B96" s="37" t="s">
         <v>306</v>
       </c>
     </row>
     <row r="97" spans="1:2" ht="135">
-      <c r="A97" s="61"/>
-      <c r="B97" s="38" t="s">
+      <c r="A97" s="64"/>
+      <c r="B97" s="37" t="s">
         <v>307</v>
       </c>
     </row>
     <row r="98" spans="1:2">
-      <c r="A98" s="61"/>
-      <c r="B98" s="37"/>
+      <c r="A98" s="64"/>
+      <c r="B98" s="36"/>
     </row>
     <row r="99" spans="1:2" ht="60">
-      <c r="A99" s="62" t="s">
+      <c r="A99" s="65" t="s">
         <v>308</v>
       </c>
-      <c r="B99" s="37" t="s">
+      <c r="B99" s="36" t="s">
         <v>309</v>
       </c>
     </row>
     <row r="100" spans="1:2" ht="45">
-      <c r="A100" s="62"/>
-      <c r="B100" s="37" t="s">
+      <c r="A100" s="65"/>
+      <c r="B100" s="36" t="s">
         <v>310</v>
       </c>
     </row>
     <row r="101" spans="1:2" ht="45">
-      <c r="A101" s="62"/>
-      <c r="B101" s="37" t="s">
+      <c r="A101" s="65"/>
+      <c r="B101" s="36" t="s">
         <v>311</v>
       </c>
     </row>
     <row r="102" spans="1:2" ht="75">
-      <c r="A102" s="61" t="s">
+      <c r="A102" s="64" t="s">
         <v>312</v>
       </c>
       <c r="B102" s="2" t="s">
@@ -13978,48 +13945,48 @@
       </c>
     </row>
     <row r="103" spans="1:2" ht="150">
-      <c r="A103" s="61"/>
+      <c r="A103" s="64"/>
       <c r="B103" s="2" t="s">
         <v>314</v>
       </c>
     </row>
     <row r="104" spans="1:2" ht="150">
-      <c r="A104" s="61"/>
+      <c r="A104" s="64"/>
       <c r="B104" s="2" t="s">
         <v>315</v>
       </c>
     </row>
     <row r="105" spans="1:2">
-      <c r="A105" s="61"/>
+      <c r="A105" s="64"/>
     </row>
     <row r="106" spans="1:2">
-      <c r="A106" s="24" t="s">
+      <c r="A106" s="23" t="s">
         <v>316</v>
       </c>
     </row>
     <row r="108" spans="1:2" ht="45">
-      <c r="A108" s="62" t="s">
+      <c r="A108" s="65" t="s">
         <v>317</v>
       </c>
-      <c r="B108" s="12" t="s">
+      <c r="B108" s="11" t="s">
         <v>318</v>
       </c>
     </row>
     <row r="109" spans="1:2">
-      <c r="A109" s="62"/>
-      <c r="B109" s="13" t="s">
+      <c r="A109" s="65"/>
+      <c r="B109" s="12" t="s">
         <v>319</v>
       </c>
     </row>
     <row r="110" spans="1:2" ht="75">
-      <c r="A110" s="62"/>
-      <c r="B110" s="12" t="s">
+      <c r="A110" s="65"/>
+      <c r="B110" s="11" t="s">
         <v>320</v>
       </c>
     </row>
     <row r="111" spans="1:2" ht="45">
-      <c r="A111" s="62"/>
-      <c r="B111" s="12" t="s">
+      <c r="A111" s="65"/>
+      <c r="B111" s="11" t="s">
         <v>321</v>
       </c>
     </row>
@@ -14032,7 +13999,7 @@
       </c>
     </row>
     <row r="113" spans="1:2" ht="60">
-      <c r="A113" s="61" t="s">
+      <c r="A113" s="64" t="s">
         <v>324</v>
       </c>
       <c r="B113" s="2" t="s">
@@ -14040,51 +14007,51 @@
       </c>
     </row>
     <row r="114" spans="1:2" ht="90">
-      <c r="A114" s="61"/>
-      <c r="B114" s="12" t="s">
+      <c r="A114" s="64"/>
+      <c r="B114" s="11" t="s">
         <v>326</v>
       </c>
     </row>
     <row r="115" spans="1:2" ht="240">
-      <c r="A115" s="61"/>
+      <c r="A115" s="64"/>
       <c r="B115" s="2" t="s">
         <v>327</v>
       </c>
     </row>
     <row r="117" spans="1:2" ht="90">
-      <c r="A117" s="61" t="s">
+      <c r="A117" s="64" t="s">
         <v>328</v>
       </c>
-      <c r="B117" s="12" t="s">
+      <c r="B117" s="11" t="s">
         <v>329</v>
       </c>
     </row>
     <row r="118" spans="1:2" ht="120">
-      <c r="A118" s="61"/>
-      <c r="B118" s="12" t="s">
+      <c r="A118" s="64"/>
+      <c r="B118" s="11" t="s">
         <v>330</v>
       </c>
     </row>
     <row r="119" spans="1:2" ht="90">
-      <c r="A119" s="61"/>
+      <c r="A119" s="64"/>
       <c r="B119" s="10" t="s">
         <v>331</v>
       </c>
     </row>
     <row r="120" spans="1:2" ht="30">
-      <c r="A120" s="61"/>
+      <c r="A120" s="64"/>
       <c r="B120" s="2" t="s">
         <v>332</v>
       </c>
     </row>
     <row r="121" spans="1:2" ht="30">
-      <c r="A121" s="61"/>
+      <c r="A121" s="64"/>
       <c r="B121" s="2" t="s">
         <v>333</v>
       </c>
     </row>
     <row r="122" spans="1:2" ht="30">
-      <c r="A122" s="61"/>
+      <c r="A122" s="64"/>
       <c r="B122" s="2" t="s">
         <v>334</v>
       </c>
@@ -14151,23 +14118,23 @@
       </c>
     </row>
     <row r="3" spans="1:3" ht="30">
-      <c r="A3" s="31" t="s">
+      <c r="A3" s="30" t="s">
         <v>339</v>
       </c>
-      <c r="B3" s="32" t="s">
+      <c r="B3" s="31" t="s">
         <v>340</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="31" t="s">
+      <c r="A4" s="30" t="s">
         <v>341</v>
       </c>
-      <c r="B4" s="32" t="s">
+      <c r="B4" s="31" t="s">
         <v>342</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="64.5" customHeight="1">
-      <c r="A5" s="59" t="s">
+      <c r="A5" s="58" t="s">
         <v>343</v>
       </c>
       <c r="B5" s="6" t="s">
@@ -14185,43 +14152,43 @@
       </c>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="74" t="s">
+      <c r="A8" s="77" t="s">
         <v>347</v>
       </c>
-      <c r="B8" s="27" t="s">
+      <c r="B8" s="26" t="s">
         <v>348</v>
       </c>
-      <c r="C8" s="77" t="s">
+      <c r="C8" s="80" t="s">
         <v>349</v>
       </c>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" s="75"/>
-      <c r="B9" s="25" t="s">
+      <c r="A9" s="78"/>
+      <c r="B9" s="24" t="s">
         <v>350</v>
       </c>
-      <c r="C9" s="75"/>
+      <c r="C9" s="78"/>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" s="75"/>
-      <c r="B10" s="27" t="s">
+      <c r="A10" s="78"/>
+      <c r="B10" s="26" t="s">
         <v>351</v>
       </c>
-      <c r="C10" s="75"/>
+      <c r="C10" s="78"/>
     </row>
     <row r="11" spans="1:3">
-      <c r="A11" s="75"/>
-      <c r="B11" s="25" t="s">
+      <c r="A11" s="78"/>
+      <c r="B11" s="24" t="s">
         <v>352</v>
       </c>
-      <c r="C11" s="75"/>
+      <c r="C11" s="78"/>
     </row>
     <row r="12" spans="1:3">
-      <c r="A12" s="76"/>
-      <c r="B12" s="27" t="s">
+      <c r="A12" s="79"/>
+      <c r="B12" s="26" t="s">
         <v>353</v>
       </c>
-      <c r="C12" s="76"/>
+      <c r="C12" s="79"/>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="5" t="s">
@@ -14291,7 +14258,7 @@
       </c>
     </row>
     <row r="28" spans="1:11">
-      <c r="B28" s="21" t="s">
+      <c r="B28" s="20" t="s">
         <v>368</v>
       </c>
       <c r="C28" s="1" t="s">
@@ -14331,13 +14298,13 @@
       </c>
     </row>
     <row r="34" spans="1:3" ht="360">
-      <c r="A34" s="30" t="s">
+      <c r="A34" s="29" t="s">
         <v>378</v>
       </c>
       <c r="B34" s="6" t="s">
         <v>379</v>
       </c>
-      <c r="C34" s="33" t="s">
+      <c r="C34" s="32" t="s">
         <v>380</v>
       </c>
     </row>
@@ -14395,19 +14362,19 @@
       </c>
     </row>
     <row r="43" spans="1:3" ht="180">
-      <c r="A43" s="63" t="s">
+      <c r="A43" s="66" t="s">
         <v>393</v>
       </c>
-      <c r="B43" s="20" t="s">
+      <c r="B43" s="19" t="s">
         <v>394</v>
       </c>
-      <c r="C43" s="12" t="s">
+      <c r="C43" s="11" t="s">
         <v>395</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="120">
-      <c r="A44" s="63"/>
-      <c r="B44" s="20" t="s">
+      <c r="A44" s="66"/>
+      <c r="B44" s="19" t="s">
         <v>393</v>
       </c>
       <c r="C44" s="2" t="s">
@@ -14415,8 +14382,8 @@
       </c>
     </row>
     <row r="45" spans="1:3" ht="180">
-      <c r="A45" s="63"/>
-      <c r="B45" s="20" t="s">
+      <c r="A45" s="66"/>
+      <c r="B45" s="19" t="s">
         <v>397</v>
       </c>
       <c r="C45" s="2" t="s">
@@ -14424,8 +14391,8 @@
       </c>
     </row>
     <row r="46" spans="1:3" ht="30">
-      <c r="A46" s="63"/>
-      <c r="B46" s="20" t="s">
+      <c r="A46" s="66"/>
+      <c r="B46" s="19" t="s">
         <v>399</v>
       </c>
       <c r="C46" s="2" t="s">
@@ -14469,7 +14436,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="30">
-      <c r="A1" s="78" t="s">
+      <c r="A1" s="81" t="s">
         <v>401</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -14477,128 +14444,128 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="90">
-      <c r="A2" s="79"/>
-      <c r="B2" s="12" t="s">
+      <c r="A2" s="82"/>
+      <c r="B2" s="11" t="s">
         <v>403</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="75">
-      <c r="A3" s="79"/>
-      <c r="B3" s="12" t="s">
+      <c r="A3" s="82"/>
+      <c r="B3" s="11" t="s">
         <v>404</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="75">
-      <c r="A4" s="79"/>
-      <c r="B4" s="12" t="s">
+      <c r="A4" s="82"/>
+      <c r="B4" s="11" t="s">
         <v>405</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="30">
-      <c r="A5" s="79"/>
-      <c r="B5" s="12" t="s">
+      <c r="A5" s="82"/>
+      <c r="B5" s="11" t="s">
         <v>406</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="135">
-      <c r="A6" s="79"/>
+      <c r="A6" s="82"/>
       <c r="B6" s="2" t="s">
         <v>407</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="18.75">
-      <c r="A7" s="79"/>
-      <c r="B7" s="29" t="s">
+      <c r="A7" s="82"/>
+      <c r="B7" s="28" t="s">
         <v>408</v>
       </c>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="79"/>
-      <c r="C8" s="30"/>
+      <c r="A8" s="82"/>
+      <c r="C8" s="29"/>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" s="79"/>
+      <c r="A9" s="82"/>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" s="79"/>
+      <c r="A10" s="82"/>
     </row>
     <row r="11" spans="1:3">
-      <c r="A11" s="79"/>
+      <c r="A11" s="82"/>
     </row>
     <row r="12" spans="1:3">
-      <c r="A12" s="79"/>
+      <c r="A12" s="82"/>
     </row>
     <row r="13" spans="1:3">
-      <c r="A13" s="79"/>
+      <c r="A13" s="82"/>
     </row>
     <row r="14" spans="1:3">
-      <c r="A14" s="79"/>
+      <c r="A14" s="82"/>
     </row>
     <row r="15" spans="1:3">
-      <c r="A15" s="79"/>
+      <c r="A15" s="82"/>
     </row>
     <row r="16" spans="1:3">
-      <c r="A16" s="79"/>
+      <c r="A16" s="82"/>
     </row>
     <row r="17" spans="1:1">
-      <c r="A17" s="79"/>
+      <c r="A17" s="82"/>
     </row>
     <row r="18" spans="1:1">
-      <c r="A18" s="79"/>
+      <c r="A18" s="82"/>
     </row>
     <row r="19" spans="1:1">
-      <c r="A19" s="79"/>
+      <c r="A19" s="82"/>
     </row>
     <row r="20" spans="1:1">
-      <c r="A20" s="79"/>
+      <c r="A20" s="82"/>
     </row>
     <row r="21" spans="1:1">
-      <c r="A21" s="79"/>
+      <c r="A21" s="82"/>
     </row>
     <row r="22" spans="1:1">
-      <c r="A22" s="79"/>
+      <c r="A22" s="82"/>
     </row>
     <row r="23" spans="1:1">
-      <c r="A23" s="79"/>
+      <c r="A23" s="82"/>
     </row>
     <row r="24" spans="1:1">
-      <c r="A24" s="79"/>
+      <c r="A24" s="82"/>
     </row>
     <row r="25" spans="1:1">
-      <c r="A25" s="79"/>
+      <c r="A25" s="82"/>
     </row>
     <row r="26" spans="1:1">
-      <c r="A26" s="79"/>
+      <c r="A26" s="82"/>
     </row>
     <row r="27" spans="1:1">
-      <c r="A27" s="79"/>
+      <c r="A27" s="82"/>
     </row>
     <row r="28" spans="1:1">
-      <c r="A28" s="79"/>
+      <c r="A28" s="82"/>
     </row>
     <row r="29" spans="1:1">
-      <c r="A29" s="79"/>
+      <c r="A29" s="82"/>
     </row>
     <row r="30" spans="1:1">
-      <c r="A30" s="79"/>
+      <c r="A30" s="82"/>
     </row>
     <row r="31" spans="1:1">
-      <c r="A31" s="79"/>
+      <c r="A31" s="82"/>
     </row>
     <row r="32" spans="1:1">
-      <c r="A32" s="79"/>
+      <c r="A32" s="82"/>
     </row>
     <row r="33" spans="1:2">
-      <c r="A33" s="79"/>
+      <c r="A33" s="82"/>
     </row>
     <row r="34" spans="1:2">
-      <c r="A34" s="79"/>
+      <c r="A34" s="82"/>
     </row>
     <row r="35" spans="1:2">
-      <c r="A35" s="79"/>
+      <c r="A35" s="82"/>
     </row>
     <row r="36" spans="1:2" ht="45">
-      <c r="A36" s="79" t="s">
+      <c r="A36" s="82" t="s">
         <v>409</v>
       </c>
       <c r="B36" s="2" t="s">
@@ -14606,88 +14573,88 @@
       </c>
     </row>
     <row r="37" spans="1:2">
-      <c r="A37" s="79"/>
-      <c r="B37" s="13" t="s">
+      <c r="A37" s="82"/>
+      <c r="B37" s="12" t="s">
         <v>411</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="18.75">
-      <c r="A38" s="79"/>
-      <c r="B38" s="29" t="s">
+      <c r="A38" s="82"/>
+      <c r="B38" s="28" t="s">
         <v>408</v>
       </c>
     </row>
     <row r="39" spans="1:2">
-      <c r="A39" s="79"/>
+      <c r="A39" s="82"/>
     </row>
     <row r="40" spans="1:2">
-      <c r="A40" s="79"/>
+      <c r="A40" s="82"/>
     </row>
     <row r="41" spans="1:2">
-      <c r="A41" s="79"/>
+      <c r="A41" s="82"/>
     </row>
     <row r="42" spans="1:2">
-      <c r="A42" s="79"/>
+      <c r="A42" s="82"/>
     </row>
     <row r="43" spans="1:2">
-      <c r="A43" s="79"/>
+      <c r="A43" s="82"/>
     </row>
     <row r="44" spans="1:2">
-      <c r="A44" s="79"/>
+      <c r="A44" s="82"/>
     </row>
     <row r="45" spans="1:2">
-      <c r="A45" s="79"/>
+      <c r="A45" s="82"/>
     </row>
     <row r="46" spans="1:2">
-      <c r="A46" s="79"/>
+      <c r="A46" s="82"/>
     </row>
     <row r="47" spans="1:2">
-      <c r="A47" s="79"/>
+      <c r="A47" s="82"/>
     </row>
     <row r="48" spans="1:2">
-      <c r="A48" s="79"/>
+      <c r="A48" s="82"/>
     </row>
     <row r="49" spans="1:1">
-      <c r="A49" s="79"/>
+      <c r="A49" s="82"/>
     </row>
     <row r="50" spans="1:1">
-      <c r="A50" s="79"/>
+      <c r="A50" s="82"/>
     </row>
     <row r="51" spans="1:1">
-      <c r="A51" s="79"/>
+      <c r="A51" s="82"/>
     </row>
     <row r="52" spans="1:1">
-      <c r="A52" s="79"/>
+      <c r="A52" s="82"/>
     </row>
     <row r="53" spans="1:1">
-      <c r="A53" s="79"/>
+      <c r="A53" s="82"/>
     </row>
     <row r="54" spans="1:1">
-      <c r="A54" s="79"/>
+      <c r="A54" s="82"/>
     </row>
     <row r="55" spans="1:1">
-      <c r="A55" s="79"/>
+      <c r="A55" s="82"/>
     </row>
     <row r="56" spans="1:1">
-      <c r="A56" s="79"/>
+      <c r="A56" s="82"/>
     </row>
     <row r="57" spans="1:1">
-      <c r="A57" s="79"/>
+      <c r="A57" s="82"/>
     </row>
     <row r="58" spans="1:1">
-      <c r="A58" s="79"/>
+      <c r="A58" s="82"/>
     </row>
     <row r="59" spans="1:1">
-      <c r="A59" s="79"/>
+      <c r="A59" s="82"/>
     </row>
     <row r="60" spans="1:1">
-      <c r="A60" s="79"/>
+      <c r="A60" s="82"/>
     </row>
     <row r="61" spans="1:1">
-      <c r="A61" s="79"/>
+      <c r="A61" s="82"/>
     </row>
     <row r="62" spans="1:1">
-      <c r="A62" s="79"/>
+      <c r="A62" s="82"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -14728,57 +14695,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="24" t="s">
         <v>412</v>
       </c>
-      <c r="B1" s="80" t="s">
+      <c r="B1" s="83" t="s">
         <v>413</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="C1" s="25" t="s">
         <v>414</v>
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="26" t="s">
         <v>415</v>
       </c>
-      <c r="B2" s="75"/>
-      <c r="C2" s="27"/>
+      <c r="B2" s="78"/>
+      <c r="C2" s="26"/>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="24" t="s">
         <v>416</v>
       </c>
-      <c r="B3" s="75"/>
-      <c r="C3" s="25"/>
+      <c r="B3" s="78"/>
+      <c r="C3" s="24"/>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="26" t="s">
         <v>417</v>
       </c>
-      <c r="B4" s="75"/>
-      <c r="C4" s="27"/>
+      <c r="B4" s="78"/>
+      <c r="C4" s="26"/>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="25" t="s">
+      <c r="A5" s="24" t="s">
         <v>418</v>
       </c>
-      <c r="B5" s="75"/>
-      <c r="C5" s="25"/>
+      <c r="B5" s="78"/>
+      <c r="C5" s="24"/>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="27" t="s">
+      <c r="A6" s="26" t="s">
         <v>419</v>
       </c>
-      <c r="B6" s="75"/>
-      <c r="C6" s="27"/>
+      <c r="B6" s="78"/>
+      <c r="C6" s="26"/>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="25" t="s">
+      <c r="A7" s="24" t="s">
         <v>420</v>
       </c>
-      <c r="B7" s="76"/>
-      <c r="C7" s="25"/>
+      <c r="B7" s="79"/>
+      <c r="C7" s="24"/>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
@@ -14905,7 +14872,7 @@
       </c>
     </row>
     <row r="11" spans="1:4" ht="75">
-      <c r="A11" s="72" t="s">
+      <c r="A11" s="75" t="s">
         <v>443</v>
       </c>
       <c r="B11" s="2" t="s">
@@ -14919,7 +14886,7 @@
       </c>
     </row>
     <row r="12" spans="1:4" ht="90">
-      <c r="A12" s="72"/>
+      <c r="A12" s="75"/>
       <c r="B12" s="2" t="s">
         <v>447</v>
       </c>

</xml_diff>